<commit_message>
Rework to Macro and All
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaar_000\Documents\GitHub\MatrixPepco\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Audit Master" sheetId="1" r:id="rId1"/>
@@ -116,7 +121,7 @@
     <definedName name="U_Lamps">#REF!</definedName>
     <definedName name="Watts_Saved">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -249,7 +254,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="10">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
@@ -5544,7 +5549,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5568,7 +5573,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Project Data"/>
@@ -20865,7 +20870,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20897,9 +20902,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20931,6 +20937,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -21106,29 +21113,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="9" customWidth="1"/>
     <col min="4" max="4" width="43" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="11" customWidth="1"/>
     <col min="6" max="6" width="41" style="9" customWidth="1"/>
     <col min="7" max="7" width="12" style="11" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="37" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
@@ -21268,7 +21275,7 @@
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" thickBot="1">
+    <row r="11" spans="1:10" ht="12.6" thickBot="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -21294,7 +21301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="13" customFormat="1" ht="100.9" customHeight="1">
+    <row r="13" spans="1:10" s="13" customFormat="1" ht="100.95" customHeight="1">
       <c r="A13" s="53" t="s">
         <v>10</v>
       </c>
@@ -21326,7 +21333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75">
+    <row r="14" spans="1:10" ht="18">
       <c r="A14" s="27">
         <v>1</v>
       </c>
@@ -21340,7 +21347,7 @@
       <c r="I14" s="40"/>
       <c r="J14" s="56"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75">
+    <row r="15" spans="1:10" ht="18">
       <c r="A15" s="7">
         <f>A14+1</f>
         <v>2</v>
@@ -21355,7 +21362,7 @@
       <c r="I15" s="41"/>
       <c r="J15" s="56"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75">
+    <row r="16" spans="1:10" ht="18">
       <c r="A16" s="7">
         <f t="shared" ref="A16:A23" si="0">A15+1</f>
         <v>3</v>
@@ -21370,7 +21377,7 @@
       <c r="I16" s="42"/>
       <c r="J16" s="57"/>
     </row>
-    <row r="17" spans="1:10" ht="25.9" customHeight="1">
+    <row r="17" spans="1:10" ht="25.95" customHeight="1">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -21385,7 +21392,7 @@
       <c r="I17" s="42"/>
       <c r="J17" s="57"/>
     </row>
-    <row r="18" spans="1:10" ht="25.9" customHeight="1">
+    <row r="18" spans="1:10" ht="25.95" customHeight="1">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -21400,7 +21407,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="57"/>
     </row>
-    <row r="19" spans="1:10" ht="25.9" customHeight="1">
+    <row r="19" spans="1:10" ht="25.95" customHeight="1">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -21415,7 +21422,7 @@
       <c r="I19" s="43"/>
       <c r="J19" s="57"/>
     </row>
-    <row r="20" spans="1:10" ht="25.9" customHeight="1">
+    <row r="20" spans="1:10" ht="25.95" customHeight="1">
       <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -21430,7 +21437,7 @@
       <c r="I20" s="43"/>
       <c r="J20" s="57"/>
     </row>
-    <row r="21" spans="1:10" ht="25.9" customHeight="1">
+    <row r="21" spans="1:10" ht="25.95" customHeight="1">
       <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -21445,7 +21452,7 @@
       <c r="I21" s="43"/>
       <c r="J21" s="57"/>
     </row>
-    <row r="22" spans="1:10" ht="25.9" customHeight="1">
+    <row r="22" spans="1:10" ht="25.95" customHeight="1">
       <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -21565,7 +21572,7 @@
       <c r="G30" s="74"/>
       <c r="H30" s="74"/>
     </row>
-    <row r="31" spans="1:10" s="28" customFormat="1" ht="15.75" thickBot="1">
+    <row r="31" spans="1:10" s="28" customFormat="1" ht="15" thickBot="1">
       <c r="A31" s="70"/>
       <c r="B31" s="70"/>
       <c r="C31" s="25"/>
@@ -21575,7 +21582,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
     </row>
-    <row r="32" spans="1:10" s="28" customFormat="1" ht="15.75">
+    <row r="32" spans="1:10" s="28" customFormat="1" ht="15.6">
       <c r="A32" s="65" t="s">
         <v>17</v>
       </c>
@@ -21589,7 +21596,7 @@
       <c r="G32" s="66"/>
       <c r="I32" s="29"/>
     </row>
-    <row r="33" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="33" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A33" s="24"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -21598,7 +21605,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="34" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A34" s="24"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -21607,7 +21614,7 @@
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="35" spans="1:9" s="28" customFormat="1" ht="16.5" thickBot="1">
+    <row r="35" spans="1:9" s="28" customFormat="1" ht="16.2" thickBot="1">
       <c r="A35" s="69"/>
       <c r="B35" s="69"/>
       <c r="C35" s="23"/>
@@ -21618,7 +21625,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="36" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A36" s="65" t="s">
         <v>19</v>
       </c>
@@ -21631,7 +21638,7 @@
       </c>
       <c r="G36" s="66"/>
     </row>
-    <row r="37" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="37" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A37" s="24"/>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
@@ -21640,7 +21647,7 @@
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A38" s="24"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -21649,7 +21656,7 @@
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:9" s="28" customFormat="1" ht="16.5" thickBot="1">
+    <row r="39" spans="1:9" s="28" customFormat="1" ht="16.2" thickBot="1">
       <c r="A39" s="69"/>
       <c r="B39" s="69"/>
       <c r="C39" s="23"/>
@@ -21660,7 +21667,7 @@
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
     </row>
-    <row r="40" spans="1:9" s="28" customFormat="1" ht="15.75">
+    <row r="40" spans="1:9" s="28" customFormat="1" ht="15.6">
       <c r="A40" s="65" t="s">
         <v>20</v>
       </c>
@@ -21723,7 +21730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -21731,7 +21738,7 @@
       <selection activeCell="A2" sqref="A2:IV11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="19"/>
@@ -21744,7 +21751,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="70"/>
       <c r="B2" s="70"/>
       <c r="C2" s="29"/>
@@ -21792,7 +21799,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="29"/>
@@ -21840,7 +21847,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="70"/>
       <c r="B10" s="70"/>
       <c r="C10" s="29"/>

</xml_diff>

<commit_message>
Added 50 fields to indoor lighting
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaar_000\Documents\GitHub\MatrixPepco\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800"/>
   </bookViews>
@@ -121,7 +116,7 @@
     <definedName name="U_Lamps">#REF!</definedName>
     <definedName name="Watts_Saved">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -254,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
@@ -583,15 +578,13 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="14"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1125,7 +1118,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2060">
+  <cellStyleXfs count="2059">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3225,9 +3218,8 @@
     <xf numFmtId="37" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="46" fillId="0" borderId="18" applyProtection="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3266,9 +3258,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3371,56 +3360,11 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="24" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="6" borderId="2" xfId="2059" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3435,6 +3379,18 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3447,8 +3403,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="52" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2060">
+  <cellStyles count="2059">
     <cellStyle name="20% - Accent1 2" xfId="33"/>
     <cellStyle name="20% - Accent2 2" xfId="34"/>
     <cellStyle name="20% - Accent3 2" xfId="35"/>
@@ -3528,7 +3508,6 @@
     <cellStyle name="Heading2 3" xfId="93"/>
     <cellStyle name="Hidden" xfId="94"/>
     <cellStyle name="HIGHLIGHT" xfId="95"/>
-    <cellStyle name="Hyperlink" xfId="2059" builtinId="8"/>
     <cellStyle name="Input [yellow]" xfId="96"/>
     <cellStyle name="Input 2" xfId="97"/>
     <cellStyle name="Linked Cell 2" xfId="98"/>
@@ -5549,7 +5528,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5573,7 +5552,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Project Data"/>
@@ -20870,7 +20849,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20902,10 +20881,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20937,7 +20915,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -21113,29 +21090,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="43" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="11" customWidth="1"/>
     <col min="6" max="6" width="41" style="9" customWidth="1"/>
     <col min="7" max="7" width="12" style="11" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="37" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1">
@@ -21145,7 +21122,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="I1" s="22"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="30.6" customHeight="1">
       <c r="A2" s="4"/>
@@ -21153,7 +21130,7 @@
       <c r="C2" s="4"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -21163,7 +21140,7 @@
       <c r="C3" s="4"/>
       <c r="E3" s="15"/>
       <c r="F3" s="17"/>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -21171,99 +21148,99 @@
       <c r="A4" s="5"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
       <c r="J4" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="63" t="s">
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="63" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
     </row>
     <row r="7" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="71"/>
+      <c r="C7" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="63" t="s">
+      <c r="D7" s="73"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
     </row>
     <row r="8" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="71" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="63" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:10" ht="30.6" customHeight="1">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="68"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="72" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="73"/>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="74"/>
+      <c r="F9" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
     </row>
     <row r="10" spans="1:10" ht="30.6" customHeight="1">
       <c r="A10" s="16"/>
@@ -21275,7 +21252,7 @@
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:10" ht="12.6" thickBot="1">
+    <row r="11" spans="1:10" ht="12.75" thickBot="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -21288,410 +21265,407 @@
     <row r="12" spans="1:10" s="13" customFormat="1" ht="15" customHeight="1" thickTop="1">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="75" t="s">
+      <c r="E12" s="61"/>
+      <c r="F12" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="44" t="s">
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="13" customFormat="1" ht="100.95" customHeight="1">
-      <c r="A13" s="53" t="s">
+    <row r="13" spans="1:10" s="13" customFormat="1" ht="100.9" customHeight="1">
+      <c r="A13" s="52" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="32" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="39" t="s">
+      <c r="I13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18">
-      <c r="A14" s="27">
+    <row r="14" spans="1:10" ht="18.75">
+      <c r="A14" s="26">
         <v>1</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="56"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="55"/>
     </row>
-    <row r="15" spans="1:10" ht="18">
+    <row r="15" spans="1:10" ht="18.75">
       <c r="A15" s="7">
         <f>A14+1</f>
         <v>2</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="55"/>
     </row>
-    <row r="16" spans="1:10" ht="18">
+    <row r="16" spans="1:10" ht="18.75">
       <c r="A16" s="7">
         <f t="shared" ref="A16:A23" si="0">A15+1</f>
         <v>3</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="57"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="56"/>
     </row>
-    <row r="17" spans="1:10" ht="25.95" customHeight="1">
+    <row r="17" spans="1:10" ht="25.9" customHeight="1">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="57"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="56"/>
     </row>
-    <row r="18" spans="1:10" ht="25.95" customHeight="1">
+    <row r="18" spans="1:10" ht="25.9" customHeight="1">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="57"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="56"/>
     </row>
-    <row r="19" spans="1:10" ht="25.95" customHeight="1">
+    <row r="19" spans="1:10" ht="25.9" customHeight="1">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="57"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="56"/>
     </row>
-    <row r="20" spans="1:10" ht="25.95" customHeight="1">
+    <row r="20" spans="1:10" ht="25.9" customHeight="1">
       <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="57"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="56"/>
     </row>
-    <row r="21" spans="1:10" ht="25.95" customHeight="1">
+    <row r="21" spans="1:10" ht="25.9" customHeight="1">
       <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="57"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="56"/>
     </row>
-    <row r="22" spans="1:10" ht="25.95" customHeight="1">
+    <row r="22" spans="1:10" ht="25.9" customHeight="1">
       <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="57"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:10" ht="31.5" customHeight="1">
       <c r="A23" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="57"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="56"/>
     </row>
     <row r="24" spans="1:10" ht="24" customHeight="1">
-      <c r="A24" s="30"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
     </row>
     <row r="25" spans="1:10" ht="24" customHeight="1">
-      <c r="A25" s="30"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52" t="s">
+      <c r="C25" s="50"/>
+      <c r="D25" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" spans="1:10" ht="24" customHeight="1">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52" t="s">
+      <c r="C26" s="50"/>
+      <c r="D26" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
     </row>
     <row r="27" spans="1:10" ht="24" customHeight="1">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
     </row>
     <row r="28" spans="1:10" ht="24" customHeight="1">
-      <c r="A28" s="30"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52" t="s">
+      <c r="C28" s="50"/>
+      <c r="D28" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
     </row>
     <row r="29" spans="1:10" ht="24" customHeight="1">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52" t="s">
+      <c r="C29" s="50"/>
+      <c r="D29" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
     </row>
-    <row r="31" spans="1:10" s="28" customFormat="1" ht="15" thickBot="1">
-      <c r="A31" s="70"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
+    <row r="31" spans="1:10" s="27" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A31" s="64"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:10" s="28" customFormat="1" ht="15.6">
-      <c r="A32" s="65" t="s">
+    <row r="32" spans="1:10" s="27" customFormat="1" ht="15.75">
+      <c r="A32" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="66" t="s">
+      <c r="B32" s="57"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="66"/>
-      <c r="I32" s="29"/>
+      <c r="G32" s="62"/>
+      <c r="I32" s="28"/>
     </row>
-    <row r="33" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
+    <row r="33" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
-    <row r="34" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
+    <row r="34" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
     </row>
-    <row r="35" spans="1:9" s="28" customFormat="1" ht="16.2" thickBot="1">
-      <c r="A35" s="69"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+    <row r="35" spans="1:9" s="27" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
-    <row r="36" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A36" s="65" t="s">
+    <row r="36" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A36" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="66" t="s">
+      <c r="B36" s="57"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="66"/>
+      <c r="G36" s="62"/>
     </row>
-    <row r="37" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+    <row r="37" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
     </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
+    <row r="38" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
     </row>
-    <row r="39" spans="1:9" s="28" customFormat="1" ht="16.2" thickBot="1">
-      <c r="A39" s="69"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
+    <row r="39" spans="1:9" s="27" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A39" s="63"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" s="28" customFormat="1" ht="15.6">
-      <c r="A40" s="65" t="s">
+    <row r="40" spans="1:9" s="27" customFormat="1" ht="15.75">
+      <c r="A40" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="66" t="s">
+      <c r="B40" s="57"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="66"/>
+      <c r="G40" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E8:F8"/>
+  <mergeCells count="31">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="A5:B5"/>
@@ -21708,16 +21682,14 @@
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" display="carrie.giles@matrixescorp.com"/>
@@ -21730,7 +21702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -21738,7 +21710,7 @@
       <selection activeCell="A2" sqref="A2:IV11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="19"/>
@@ -21751,27 +21723,27 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="80" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="81"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -21799,27 +21771,27 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1">
-      <c r="A6" s="70"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="80" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -21847,27 +21819,27 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1">
-      <c r="A10" s="70"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="80" t="s">
+      <c r="B11" s="67"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="81"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -21875,18 +21847,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Work order and 53 to 133 bug
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaar_000\Documents\GitHub\MatrixPepco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ala\Documents\GitHub\MatrixPepco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Audit Master" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
   <si>
     <t>Business Name:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number: </t>
   </si>
   <si>
     <t>Building Address:</t>
@@ -549,6 +546,9 @@
   <si>
     <t>Combo</t>
   </si>
+  <si>
+    <t>Phone Number:</t>
+  </si>
 </sst>
 </file>
 
@@ -948,11 +948,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
@@ -964,6 +966,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1172,7 +1175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="70">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -1839,74 +1842,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -4091,7 +4026,7 @@
     <xf numFmtId="3" fontId="44" fillId="0" borderId="18" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4136,16 +4071,16 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4252,9 +4187,9 @@
     <xf numFmtId="0" fontId="54" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="62" fillId="34" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="62" fillId="34" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4375,7 +4310,7 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4383,20 +4318,30 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="49" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="48" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4475,7 +4420,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4517,24 +4462,6 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4562,19 +4489,6 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="49" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2059">
     <cellStyle name="20% - Accent1 2" xfId="33"/>
@@ -22295,32 +22209,32 @@
   <dimension ref="A1:IM93"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" style="39" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="36.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" style="1" customWidth="1"/>
-    <col min="13" max="25" width="9.109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" style="1" customWidth="1"/>
-    <col min="27" max="247" width="9.109375" style="1" customWidth="1"/>
-    <col min="248" max="16384" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="41" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" customWidth="1"/>
+    <col min="13" max="25" width="9.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" style="1" customWidth="1"/>
+    <col min="27" max="247" width="9.140625" style="1" customWidth="1"/>
+    <col min="248" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="21.6" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="33"/>
@@ -22335,29 +22249,29 @@
     </row>
     <row r="2" spans="1:27" ht="24" customHeight="1">
       <c r="A2" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
       <c r="F2" s="40"/>
       <c r="K2" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="29"/>
     </row>
-    <row r="3" spans="1:27" ht="19.2" customHeight="1">
+    <row r="3" spans="1:27" ht="19.149999999999999" customHeight="1">
       <c r="A3" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="F3" s="40"/>
       <c r="K3" s="6"/>
-      <c r="R3" s="131"/>
+      <c r="R3" s="130"/>
     </row>
     <row r="4" spans="1:27" ht="24" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
@@ -22365,105 +22279,105 @@
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
       <c r="K4" s="6"/>
-      <c r="R4" s="131"/>
+      <c r="R4" s="130"/>
     </row>
-    <row r="5" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A5" s="154" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
+    <row r="5" spans="1:27" ht="24.4" customHeight="1">
+      <c r="A5" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="159"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
       <c r="G5" s="44" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
       <c r="K5" s="46"/>
       <c r="L5" s="47"/>
-      <c r="R5" s="136"/>
+      <c r="R5" s="135"/>
     </row>
-    <row r="6" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A6" s="154" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
+    <row r="6" spans="1:27" ht="24.4" customHeight="1">
+      <c r="A6" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="159"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
       <c r="G6" s="44"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
       <c r="J6" s="45"/>
       <c r="K6" s="46"/>
       <c r="L6" s="47"/>
-      <c r="R6" s="136"/>
+      <c r="R6" s="135"/>
     </row>
-    <row r="7" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A7" s="154" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="155"/>
-      <c r="C7" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
+    <row r="7" spans="1:27" ht="24.4" customHeight="1">
+      <c r="A7" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="159"/>
+      <c r="C7" s="149" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="149"/>
+      <c r="E7" s="149"/>
+      <c r="F7" s="149"/>
       <c r="G7" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="48"/>
       <c r="I7" s="48"/>
       <c r="J7" s="48"/>
       <c r="K7" s="49"/>
       <c r="L7" s="50"/>
-      <c r="R7" s="136"/>
-      <c r="AA7" s="131"/>
+      <c r="R7" s="135"/>
+      <c r="AA7" s="130"/>
     </row>
-    <row r="8" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A8" s="154" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="155"/>
-      <c r="C8" s="146" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="146"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
+    <row r="8" spans="1:27" ht="24.4" customHeight="1">
+      <c r="A8" s="158" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="159"/>
+      <c r="C8" s="150" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="150"/>
+      <c r="E8" s="150"/>
+      <c r="F8" s="150"/>
       <c r="G8" s="51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="48"/>
       <c r="I8" s="48"/>
       <c r="J8" s="48"/>
       <c r="K8" s="49"/>
       <c r="L8" s="50"/>
-      <c r="R8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="R8" s="130"/>
+      <c r="AA8" s="130"/>
     </row>
-    <row r="9" spans="1:27" ht="24.45" hidden="1" customHeight="1">
-      <c r="A9" s="192"/>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="195"/>
+    <row r="9" spans="1:27" ht="24.4" hidden="1" customHeight="1">
+      <c r="A9" s="136"/>
+      <c r="B9" s="137"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="139"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="196"/>
+      <c r="K9" s="140"/>
       <c r="L9" s="50"/>
-      <c r="R9" s="131"/>
-      <c r="AA9" s="131"/>
+      <c r="R9" s="130"/>
+      <c r="AA9" s="130"/>
     </row>
-    <row r="10" spans="1:27" ht="24.45" customHeight="1">
+    <row r="10" spans="1:27" ht="24.4" customHeight="1">
       <c r="A10" s="52"/>
       <c r="B10" s="53"/>
       <c r="C10" s="53"/>
@@ -22473,122 +22387,122 @@
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
       <c r="K10" s="6"/>
-      <c r="R10" s="131"/>
-      <c r="AA10" s="131"/>
+      <c r="R10" s="130"/>
+      <c r="AA10" s="130"/>
     </row>
-    <row r="11" spans="1:27" ht="10.199999999999999" customHeight="1" thickBot="1">
+    <row r="11" spans="1:27" ht="10.15" customHeight="1" thickBot="1">
       <c r="A11" s="56"/>
       <c r="B11" s="38"/>
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
       <c r="G11" s="2"/>
       <c r="K11" s="6"/>
-      <c r="R11" s="131"/>
-      <c r="AA11" s="131"/>
+      <c r="R11" s="130"/>
+      <c r="AA11" s="130"/>
     </row>
     <row r="12" spans="1:27" s="3" customFormat="1" ht="12" customHeight="1" thickTop="1">
       <c r="A12" s="58"/>
       <c r="B12" s="59"/>
       <c r="C12" s="15"/>
       <c r="D12" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="61"/>
+      <c r="F12" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="147" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
+      <c r="G12" s="155"/>
+      <c r="H12" s="155"/>
       <c r="I12" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="147" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="148"/>
+        <v>19</v>
+      </c>
+      <c r="J12" s="151" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="152"/>
       <c r="L12" s="63"/>
-      <c r="AA12" s="131"/>
+      <c r="AA12" s="130"/>
     </row>
     <row r="13" spans="1:27" s="3" customFormat="1" ht="57" customHeight="1">
       <c r="A13" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="67" t="s">
         <v>7</v>
-      </c>
-      <c r="B13" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>8</v>
       </c>
       <c r="E13" s="67"/>
       <c r="F13" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="69" t="s">
+      <c r="I13" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="70" t="s">
-        <v>10</v>
-      </c>
       <c r="J13" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="134" t="s">
-        <v>69</v>
-      </c>
-      <c r="M13" s="134" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" s="134" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="133" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" s="133" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="133" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="133" t="s">
+        <v>81</v>
+      </c>
+      <c r="P13" s="134" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q13" s="134" t="s">
+        <v>112</v>
+      </c>
+      <c r="R13" s="134" t="s">
+        <v>114</v>
+      </c>
+      <c r="S13" s="133" t="s">
+        <v>117</v>
+      </c>
+      <c r="T13" s="134" t="s">
+        <v>122</v>
+      </c>
+      <c r="U13" s="134" t="s">
+        <v>129</v>
+      </c>
+      <c r="V13" s="134" t="s">
+        <v>136</v>
+      </c>
+      <c r="W13" s="133" t="s">
         <v>78</v>
       </c>
-      <c r="O13" s="134" t="s">
-        <v>82</v>
-      </c>
-      <c r="P13" s="135" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="135" t="s">
-        <v>113</v>
-      </c>
-      <c r="R13" s="135" t="s">
-        <v>115</v>
-      </c>
-      <c r="S13" s="134" t="s">
-        <v>118</v>
-      </c>
-      <c r="T13" s="135" t="s">
-        <v>123</v>
-      </c>
-      <c r="U13" s="135" t="s">
-        <v>130</v>
-      </c>
-      <c r="V13" s="135" t="s">
-        <v>137</v>
-      </c>
-      <c r="W13" s="134" t="s">
-        <v>79</v>
-      </c>
-      <c r="X13" s="135" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y13" s="135" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z13" s="134" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA13" s="131"/>
+      <c r="X13" s="134" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y13" s="134" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z13" s="133" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA13" s="130"/>
     </row>
-    <row r="14" spans="1:27" ht="29.4" customHeight="1">
+    <row r="14" spans="1:27" ht="29.45" customHeight="1">
       <c r="A14" s="74">
         <v>1</v>
       </c>
@@ -22667,9 +22581,9 @@
         <f>IF(OR(D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G14*1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="131"/>
+      <c r="AA14" s="130"/>
     </row>
-    <row r="15" spans="1:27" ht="29.4" customHeight="1">
+    <row r="15" spans="1:27" ht="29.45" customHeight="1">
       <c r="A15" s="74">
         <v>2</v>
       </c>
@@ -22748,9 +22662,9 @@
         <f t="shared" ref="Z15:Z78" si="14">IF(OR(D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G15*1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AA15" s="131"/>
+      <c r="AA15" s="130"/>
     </row>
-    <row r="16" spans="1:27" ht="29.4" customHeight="1">
+    <row r="16" spans="1:27" ht="29.45" customHeight="1">
       <c r="A16" s="74">
         <v>3</v>
       </c>
@@ -22824,9 +22738,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="131"/>
+      <c r="AA16" s="130"/>
     </row>
-    <row r="17" spans="1:27" ht="29.4" customHeight="1">
+    <row r="17" spans="1:27" ht="29.45" customHeight="1">
       <c r="A17" s="74">
         <v>4</v>
       </c>
@@ -22900,9 +22814,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="131"/>
+      <c r="AA17" s="130"/>
     </row>
-    <row r="18" spans="1:27" ht="29.4" customHeight="1">
+    <row r="18" spans="1:27" ht="29.45" customHeight="1">
       <c r="A18" s="74">
         <v>5</v>
       </c>
@@ -22976,9 +22890,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA18" s="131"/>
+      <c r="AA18" s="130"/>
     </row>
-    <row r="19" spans="1:27" ht="29.4" customHeight="1">
+    <row r="19" spans="1:27" ht="29.45" customHeight="1">
       <c r="A19" s="74">
         <v>6</v>
       </c>
@@ -23052,9 +22966,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="131"/>
+      <c r="AA19" s="130"/>
     </row>
-    <row r="20" spans="1:27" ht="29.4" customHeight="1">
+    <row r="20" spans="1:27" ht="29.45" customHeight="1">
       <c r="A20" s="74">
         <v>7</v>
       </c>
@@ -23128,9 +23042,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA20" s="131"/>
+      <c r="AA20" s="130"/>
     </row>
-    <row r="21" spans="1:27" ht="29.4" customHeight="1">
+    <row r="21" spans="1:27" ht="29.45" customHeight="1">
       <c r="A21" s="74">
         <v>8</v>
       </c>
@@ -23204,9 +23118,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA21" s="131"/>
+      <c r="AA21" s="130"/>
     </row>
-    <row r="22" spans="1:27" ht="29.4" customHeight="1">
+    <row r="22" spans="1:27" ht="29.45" customHeight="1">
       <c r="A22" s="74">
         <v>9</v>
       </c>
@@ -23280,9 +23194,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA22" s="131"/>
+      <c r="AA22" s="130"/>
     </row>
-    <row r="23" spans="1:27" ht="29.4" customHeight="1">
+    <row r="23" spans="1:27" ht="29.45" customHeight="1">
       <c r="A23" s="74">
         <v>10</v>
       </c>
@@ -23357,7 +23271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="29.4" customHeight="1">
+    <row r="24" spans="1:27" ht="29.45" customHeight="1">
       <c r="A24" s="74">
         <v>11</v>
       </c>
@@ -23432,7 +23346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="29.4" customHeight="1">
+    <row r="25" spans="1:27" ht="29.45" customHeight="1">
       <c r="A25" s="74">
         <v>12</v>
       </c>
@@ -23507,7 +23421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="29.4" customHeight="1" thickBot="1">
+    <row r="26" spans="1:27" ht="29.45" customHeight="1" thickBot="1">
       <c r="A26" s="74">
         <v>13</v>
       </c>
@@ -23582,7 +23496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="27" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A27" s="74">
         <v>14</v>
       </c>
@@ -23657,7 +23571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="28" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A28" s="74">
         <v>15</v>
       </c>
@@ -23732,7 +23646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="29" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A29" s="74">
         <v>16</v>
       </c>
@@ -23807,7 +23721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="30" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A30" s="74">
         <v>17</v>
       </c>
@@ -23882,7 +23796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="31" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A31" s="74">
         <v>18</v>
       </c>
@@ -23957,7 +23871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="32" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A32" s="74">
         <v>19</v>
       </c>
@@ -24032,7 +23946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="33" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A33" s="74">
         <v>20</v>
       </c>
@@ -24107,7 +24021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="34" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A34" s="74">
         <v>21</v>
       </c>
@@ -24182,7 +24096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="35" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A35" s="74">
         <v>22</v>
       </c>
@@ -24257,7 +24171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="36" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A36" s="74">
         <v>23</v>
       </c>
@@ -24332,7 +24246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="37" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A37" s="74">
         <v>24</v>
       </c>
@@ -24407,7 +24321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="38" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A38" s="74">
         <v>25</v>
       </c>
@@ -24482,7 +24396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="39" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A39" s="74">
         <v>26</v>
       </c>
@@ -24557,7 +24471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="40" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A40" s="74">
         <v>27</v>
       </c>
@@ -24632,7 +24546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="41" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A41" s="74">
         <v>28</v>
       </c>
@@ -24707,7 +24621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="42" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A42" s="74">
         <v>29</v>
       </c>
@@ -24782,7 +24696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="43" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A43" s="74">
         <v>30</v>
       </c>
@@ -24857,7 +24771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="44" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A44" s="74">
         <v>31</v>
       </c>
@@ -24932,7 +24846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="45" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A45" s="74">
         <v>32</v>
       </c>
@@ -25007,7 +24921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="46" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A46" s="74">
         <v>33</v>
       </c>
@@ -25082,7 +24996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="47" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A47" s="74">
         <v>34</v>
       </c>
@@ -25157,7 +25071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="48" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A48" s="74">
         <v>35</v>
       </c>
@@ -25232,7 +25146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="49" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A49" s="74">
         <v>36</v>
       </c>
@@ -25307,7 +25221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="50" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A50" s="74">
         <v>37</v>
       </c>
@@ -25382,7 +25296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="51" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A51" s="74">
         <v>38</v>
       </c>
@@ -25456,9 +25370,9 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA51" s="131"/>
+      <c r="AA51" s="130"/>
     </row>
-    <row r="52" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="52" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A52" s="74">
         <v>39</v>
       </c>
@@ -25533,7 +25447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="53" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A53" s="74">
         <v>40</v>
       </c>
@@ -25608,7 +25522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="54" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A54" s="74">
         <v>41</v>
       </c>
@@ -25683,7 +25597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="55" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A55" s="74">
         <v>42</v>
       </c>
@@ -25758,7 +25672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="56" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A56" s="74">
         <v>43</v>
       </c>
@@ -25833,7 +25747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="57" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A57" s="74">
         <v>44</v>
       </c>
@@ -25908,7 +25822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="58" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A58" s="74">
         <v>45</v>
       </c>
@@ -25983,7 +25897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="59" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A59" s="74">
         <v>46</v>
       </c>
@@ -26058,7 +25972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="60" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A60" s="74">
         <v>47</v>
       </c>
@@ -26133,7 +26047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="61" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A61" s="74">
         <v>48</v>
       </c>
@@ -26208,7 +26122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="62" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A62" s="74">
         <v>49</v>
       </c>
@@ -26283,7 +26197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="63" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A63" s="74">
         <v>50</v>
       </c>
@@ -26358,7 +26272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="29.4" hidden="1" customHeight="1">
+    <row r="64" spans="1:27" ht="29.45" hidden="1" customHeight="1">
       <c r="A64" s="74">
         <v>51</v>
       </c>
@@ -26433,7 +26347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="65" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A65" s="74">
         <v>52</v>
       </c>
@@ -26508,7 +26422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="66" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A66" s="74">
         <v>53</v>
       </c>
@@ -26583,7 +26497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="67" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A67" s="74">
         <v>54</v>
       </c>
@@ -26658,7 +26572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="68" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A68" s="74">
         <v>55</v>
       </c>
@@ -26733,7 +26647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="69" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A69" s="74">
         <v>56</v>
       </c>
@@ -26808,7 +26722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="70" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A70" s="74">
         <v>57</v>
       </c>
@@ -26883,7 +26797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="71" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A71" s="74">
         <v>58</v>
       </c>
@@ -26958,7 +26872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="72" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A72" s="74">
         <v>59</v>
       </c>
@@ -27033,7 +26947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="73" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A73" s="74">
         <v>60</v>
       </c>
@@ -27108,7 +27022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="74" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A74" s="74">
         <v>61</v>
       </c>
@@ -27183,7 +27097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="75" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A75" s="74">
         <v>62</v>
       </c>
@@ -27258,7 +27172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="76" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A76" s="74">
         <v>63</v>
       </c>
@@ -27333,7 +27247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="77" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A77" s="74">
         <v>64</v>
       </c>
@@ -27408,7 +27322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="78" spans="1:26" ht="29.45" hidden="1" customHeight="1">
       <c r="A78" s="74">
         <v>65</v>
       </c>
@@ -27483,7 +27397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="29.4" hidden="1" customHeight="1" thickBot="1">
+    <row r="79" spans="1:26" ht="29.45" hidden="1" customHeight="1" thickBot="1">
       <c r="A79" s="74">
         <v>66</v>
       </c>
@@ -27563,150 +27477,150 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="19.2" customHeight="1" thickTop="1">
+    <row r="80" spans="1:26" ht="19.149999999999999" customHeight="1" thickTop="1">
       <c r="A80" s="93"/>
       <c r="B80" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="95" t="s">
         <v>18</v>
-      </c>
-      <c r="C80" s="95" t="s">
-        <v>19</v>
       </c>
       <c r="D80" s="95"/>
       <c r="E80" s="94"/>
       <c r="G80" s="94" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H80" s="95"/>
       <c r="I80" s="95"/>
-      <c r="L80" s="132">
+      <c r="L80" s="131">
         <f>SUM(L14:L79)</f>
         <v>0</v>
       </c>
-      <c r="M80" s="132">
+      <c r="M80" s="131">
         <f t="shared" ref="M80:N80" si="30">SUM(M14:M79)</f>
         <v>0</v>
       </c>
-      <c r="N80" s="132">
+      <c r="N80" s="131">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="O80" s="132">
+      <c r="O80" s="131">
         <f t="shared" ref="O80:Z80" si="31">SUM(O14:O79)</f>
         <v>0</v>
       </c>
-      <c r="P80" s="132">
+      <c r="P80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="Q80" s="132">
+      <c r="Q80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="R80" s="132">
+      <c r="R80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="S80" s="132">
+      <c r="S80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="T80" s="132">
+      <c r="T80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="U80" s="132">
+      <c r="U80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="V80" s="132">
+      <c r="V80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="W80" s="132">
+      <c r="W80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="X80" s="132">
+      <c r="X80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="Y80" s="132">
+      <c r="Y80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="Z80" s="132">
+      <c r="Z80" s="131">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="19.2" customHeight="1">
+    <row r="81" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A81" s="93"/>
       <c r="B81" s="96"/>
       <c r="C81" s="94" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D81" s="94"/>
       <c r="E81" s="94"/>
       <c r="G81" s="94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H81" s="94"/>
       <c r="I81" s="94"/>
       <c r="K81" s="6"/>
     </row>
-    <row r="82" spans="1:12" ht="19.2" customHeight="1">
+    <row r="82" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A82" s="93"/>
       <c r="B82" s="96"/>
       <c r="C82" s="94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D82" s="94"/>
       <c r="E82" s="94"/>
       <c r="G82" s="94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H82" s="94"/>
       <c r="I82" s="94"/>
       <c r="K82" s="6"/>
     </row>
-    <row r="83" spans="1:12" ht="19.2" customHeight="1">
+    <row r="83" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A83" s="93"/>
       <c r="B83" s="96"/>
       <c r="D83" s="94"/>
       <c r="E83" s="94"/>
       <c r="G83" s="94" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H83" s="94"/>
       <c r="I83" s="94"/>
       <c r="K83" s="6"/>
     </row>
-    <row r="84" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A84" s="158"/>
-      <c r="B84" s="159"/>
+    <row r="84" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1" thickBot="1">
+      <c r="A84" s="162"/>
+      <c r="B84" s="163"/>
       <c r="C84" s="97"/>
       <c r="D84" s="97"/>
       <c r="E84" s="97"/>
-      <c r="F84" s="159"/>
-      <c r="G84" s="159"/>
+      <c r="F84" s="163"/>
+      <c r="G84" s="163"/>
       <c r="H84" s="97"/>
       <c r="I84" s="97"/>
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A85" s="149" t="s">
-        <v>11</v>
-      </c>
-      <c r="B85" s="150"/>
+      <c r="A85" s="153" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="154"/>
       <c r="C85" s="100"/>
       <c r="D85" s="100"/>
       <c r="E85" s="100"/>
-      <c r="F85" s="150" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="150"/>
+      <c r="F85" s="154" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="154"/>
       <c r="J85" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K85" s="10"/>
       <c r="L85" s="1"/>
@@ -27719,10 +27633,10 @@
       <c r="E86" s="102"/>
       <c r="F86" s="102"/>
       <c r="G86" s="102"/>
-      <c r="J86" s="137" t="s">
-        <v>34</v>
-      </c>
-      <c r="K86" s="138"/>
+      <c r="J86" s="141" t="s">
+        <v>33</v>
+      </c>
+      <c r="K86" s="142"/>
       <c r="L86" s="30"/>
     </row>
     <row r="87" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
@@ -27733,43 +27647,43 @@
       <c r="E87" s="102"/>
       <c r="F87" s="102"/>
       <c r="G87" s="102"/>
-      <c r="J87" s="139"/>
-      <c r="K87" s="140"/>
+      <c r="J87" s="143"/>
+      <c r="K87" s="144"/>
       <c r="L87" s="30"/>
     </row>
-    <row r="88" spans="1:12" s="98" customFormat="1" ht="22.8" customHeight="1" thickBot="1">
-      <c r="A88" s="156"/>
-      <c r="B88" s="157"/>
+    <row r="88" spans="1:12" s="98" customFormat="1" ht="22.9" customHeight="1" thickBot="1">
+      <c r="A88" s="160"/>
+      <c r="B88" s="161"/>
       <c r="C88" s="103"/>
       <c r="D88" s="103"/>
       <c r="E88" s="103"/>
-      <c r="F88" s="157"/>
-      <c r="G88" s="157"/>
+      <c r="F88" s="161"/>
+      <c r="G88" s="161"/>
       <c r="H88" s="97"/>
       <c r="I88" s="97"/>
-      <c r="J88" s="141" t="s">
-        <v>35</v>
-      </c>
-      <c r="K88" s="142"/>
+      <c r="J88" s="145" t="s">
+        <v>34</v>
+      </c>
+      <c r="K88" s="146"/>
       <c r="L88" s="104"/>
     </row>
-    <row r="89" spans="1:12" s="98" customFormat="1" ht="17.399999999999999" customHeight="1">
-      <c r="A89" s="149" t="s">
-        <v>13</v>
-      </c>
-      <c r="B89" s="150"/>
+    <row r="89" spans="1:12" s="98" customFormat="1" ht="17.45" customHeight="1">
+      <c r="A89" s="153" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="154"/>
       <c r="C89" s="100"/>
       <c r="D89" s="100"/>
       <c r="E89" s="100"/>
-      <c r="F89" s="150" t="s">
-        <v>13</v>
-      </c>
-      <c r="G89" s="150"/>
-      <c r="J89" s="143"/>
-      <c r="K89" s="144"/>
+      <c r="F89" s="154" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="154"/>
+      <c r="J89" s="147"/>
+      <c r="K89" s="148"/>
       <c r="L89" s="104"/>
     </row>
-    <row r="90" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1">
+    <row r="90" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1">
       <c r="A90" s="101"/>
       <c r="B90" s="102"/>
       <c r="C90" s="102"/>
@@ -27778,7 +27692,7 @@
       <c r="F90" s="102"/>
       <c r="G90" s="102"/>
       <c r="J90" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K90" s="105"/>
       <c r="L90" s="96"/>
@@ -27794,27 +27708,27 @@
       <c r="H91" s="97"/>
       <c r="I91" s="107"/>
       <c r="J91" s="108" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K91" s="109"/>
       <c r="L91" s="110"/>
     </row>
-    <row r="92" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A92" s="152" t="s">
-        <v>14</v>
-      </c>
-      <c r="B92" s="153"/>
+    <row r="92" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1" thickBot="1">
+      <c r="A92" s="156" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" s="157"/>
       <c r="C92" s="111"/>
       <c r="D92" s="111"/>
       <c r="E92" s="111"/>
-      <c r="F92" s="153" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="153"/>
+      <c r="F92" s="157" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="157"/>
       <c r="H92" s="112"/>
       <c r="I92" s="113"/>
       <c r="J92" s="114" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K92" s="11"/>
       <c r="L92" s="1"/>
@@ -27862,7 +27776,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup scale="59" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27870,45 +27784,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" style="98" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="98" customWidth="1"/>
-    <col min="3" max="3" width="65.6640625" style="98" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="98" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="98" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" style="98" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="67.140625" style="98" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92" style="98" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="98" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="98" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="98" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="98" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" customHeight="1">
       <c r="A1" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="C1" s="120" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="120" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="120" t="s">
+      <c r="E1" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="120" t="s">
+      <c r="F1" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="120" t="s">
+      <c r="G1" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="120" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="121" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J1" s="27"/>
       <c r="K1" s="27"/>
@@ -27921,17 +27835,17 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="122" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="122" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="122" t="s">
-        <v>68</v>
       </c>
       <c r="C2" s="72" t="str">
         <f t="shared" ref="C2:C62" si="0">A2&amp;B2</f>
         <v xml:space="preserve">Interior CF 1L 13W QuadPAR 20 Integral LED Lamp </v>
       </c>
       <c r="D2" s="122" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="122">
         <v>1</v>
@@ -27942,17 +27856,17 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="122" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="72" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Interior CF 1L 23W QuadPAR 20 Integral LED Lamp </v>
       </c>
       <c r="D3" s="122" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="122">
         <v>1</v>
@@ -27963,17 +27877,17 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="122" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="122" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="122" t="s">
-        <v>72</v>
       </c>
       <c r="C4" s="72" t="str">
         <f t="shared" si="0"/>
         <v>EXIT Incandescent, (1) 20W lampEXIT Sign, LED, (1) 2W lamp, Single Sided</v>
       </c>
       <c r="D4" s="122" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="122">
         <v>1</v>
@@ -27984,17 +27898,17 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="122" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="122" t="s">
         <v>74</v>
-      </c>
-      <c r="B5" s="122" t="s">
-        <v>75</v>
       </c>
       <c r="C5" s="72" t="str">
         <f t="shared" si="0"/>
         <v>EXIT Incandescent, (2) 20W lampsEXIT Sign, LED, (2) 2W lamps, Dual Sided</v>
       </c>
       <c r="D5" s="122" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="122">
         <v>2</v>
@@ -28005,23 +27919,23 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="122" t="s">
         <v>76</v>
-      </c>
-      <c r="B6" s="122" t="s">
-        <v>77</v>
       </c>
       <c r="C6" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 24", STD lampFluorescent, (1) 24", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D6" s="122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="122">
         <v>1</v>
       </c>
       <c r="F6" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="122">
         <v>1</v>
@@ -28033,30 +27947,30 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="122" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="122" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" s="122" t="s">
-        <v>81</v>
       </c>
       <c r="C7" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 48", ES lampFluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D7" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="122">
         <v>1</v>
       </c>
       <c r="F7" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="122">
         <v>1</v>
       </c>
       <c r="H7" s="98"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -28066,30 +27980,30 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="122" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="122" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" s="122" t="s">
-        <v>84</v>
       </c>
       <c r="C8" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 48", ES lampFluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D8" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="122">
         <v>1</v>
       </c>
       <c r="F8" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="122">
         <v>1</v>
       </c>
       <c r="H8" s="98"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
@@ -28099,30 +28013,30 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="122" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="122" t="s">
         <v>86</v>
-      </c>
-      <c r="B9" s="122" t="s">
-        <v>87</v>
       </c>
       <c r="C9" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (3) 48", ES lampsFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D9" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="122">
         <v>1</v>
       </c>
       <c r="F9" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="122">
         <v>1</v>
       </c>
       <c r="H9" s="98"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="130"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
@@ -28132,30 +28046,30 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="122" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", ES lampsFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D10" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="122">
         <v>1</v>
       </c>
       <c r="F10" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="122">
         <v>1</v>
       </c>
       <c r="H10" s="98"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
@@ -28165,30 +28079,30 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="122" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="122" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="122" t="s">
-        <v>90</v>
       </c>
       <c r="C11" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", ES lampsFluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D11" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="122">
         <v>1</v>
       </c>
       <c r="F11" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="122">
         <v>1</v>
       </c>
       <c r="H11" s="98"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="130"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
@@ -28198,30 +28112,30 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="122" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", ES lampsFluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D12" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="122">
         <v>1</v>
       </c>
       <c r="F12" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="122">
         <v>1</v>
       </c>
       <c r="H12" s="98"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
@@ -28231,30 +28145,30 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="122" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 96" ES lampFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D13" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="122">
         <v>2</v>
       </c>
       <c r="F13" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="122">
         <v>1</v>
       </c>
       <c r="H13" s="98"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="131"/>
+      <c r="K13" s="130"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
@@ -28264,30 +28178,30 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="122" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 96", ES lampsFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D14" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="122">
         <v>2</v>
       </c>
       <c r="F14" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="122">
         <v>1</v>
       </c>
       <c r="H14" s="98"/>
       <c r="J14" s="27"/>
-      <c r="K14" s="131"/>
+      <c r="K14" s="130"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
@@ -28297,23 +28211,23 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="122" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 96", ES lampsFluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D15" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="122">
         <v>2</v>
       </c>
       <c r="F15" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="122">
         <v>1</v>
@@ -28330,23 +28244,23 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="122" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="122" t="s">
         <v>94</v>
-      </c>
-      <c r="B16" s="122" t="s">
-        <v>95</v>
       </c>
       <c r="C16" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 96", ES lampsFluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D16" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="122">
         <v>2</v>
       </c>
       <c r="F16" s="122" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G16" s="122">
         <v>1</v>
@@ -28363,23 +28277,23 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="122" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="122" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 96", ES lampsFluorescent, (6) 48", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D17" s="122" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="122">
         <v>6</v>
       </c>
       <c r="F17" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="122">
         <v>2</v>
@@ -28388,23 +28302,23 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 24", T-8 lamp, Standard BallastFluorescent, (1) 24", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D18" s="122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="122">
         <v>1</v>
       </c>
       <c r="F18" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="122">
         <v>1</v>
@@ -28413,23 +28327,23 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="122" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 48", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D19" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="122">
         <v>2</v>
       </c>
       <c r="F19" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" s="122">
         <v>1</v>
@@ -28446,23 +28360,23 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="122" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (1) 48", T-8 lampFluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D20" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="122">
         <v>2</v>
       </c>
       <c r="F20" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" s="122">
         <v>1</v>
@@ -28470,7 +28384,7 @@
       <c r="H20" s="98"/>
       <c r="J20" s="98"/>
       <c r="K20" s="98"/>
-      <c r="L20" s="131"/>
+      <c r="L20" s="130"/>
       <c r="M20" s="98"/>
       <c r="N20" s="98"/>
       <c r="O20" s="98"/>
@@ -28479,23 +28393,23 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="122" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="122" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D21" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="122">
         <v>2</v>
       </c>
       <c r="F21" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="122">
         <v>1</v>
@@ -28512,23 +28426,23 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="122" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="122" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 48", T-8 lampFluorescent, (1) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D22" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="122">
         <v>2</v>
       </c>
       <c r="F22" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" s="122">
         <v>1</v>
@@ -28545,23 +28459,23 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="122" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (3) 48", T-8 lampFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D23" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E23" s="122">
         <v>3</v>
       </c>
       <c r="F23" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" s="122">
         <v>1</v>
@@ -28578,23 +28492,23 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="123" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D24" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" s="123">
         <v>3</v>
       </c>
       <c r="F24" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" s="122">
         <v>1</v>
@@ -28603,23 +28517,23 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="122" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lampsFluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D25" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="123">
         <v>3</v>
       </c>
       <c r="F25" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="122">
         <v>1</v>
@@ -28628,23 +28542,23 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="122" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D26" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="123">
         <v>4</v>
       </c>
       <c r="F26" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" s="122">
         <v>1</v>
@@ -28653,23 +28567,23 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="122" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="122" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lampsFluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D27" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E27" s="123">
         <v>4</v>
       </c>
       <c r="F27" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" s="122">
         <v>1</v>
@@ -28678,23 +28592,23 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)</v>
       </c>
       <c r="D28" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="123">
         <v>4</v>
       </c>
       <c r="F28" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" s="122">
         <v>1</v>
@@ -28703,23 +28617,23 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="122" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 48", T-8 lampsFluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D29" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="123">
         <v>4</v>
       </c>
       <c r="F29" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" s="122">
         <v>1</v>
@@ -28728,23 +28642,23 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="122" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 96", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D30" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="122">
         <v>4</v>
       </c>
       <c r="F30" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" s="122">
         <v>1</v>
@@ -28753,23 +28667,23 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="122" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) 96", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D31" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="122">
         <v>4</v>
       </c>
       <c r="F31" s="122" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" s="122">
         <v>1</v>
@@ -28778,23 +28692,23 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="122" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="122" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 96", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
       </c>
       <c r="D32" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="122">
         <v>4</v>
       </c>
       <c r="F32" s="122" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G32" s="122">
         <v>1</v>
@@ -28803,23 +28717,23 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="122" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="122" t="s">
         <v>109</v>
-      </c>
-      <c r="B33" s="122" t="s">
-        <v>110</v>
       </c>
       <c r="C33" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (4) 96", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D33" s="122" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" s="122">
         <v>6</v>
       </c>
       <c r="F33" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="122">
         <v>2</v>
@@ -28828,23 +28742,23 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="122" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="122" t="s">
         <v>111</v>
-      </c>
-      <c r="B34" s="122" t="s">
-        <v>112</v>
       </c>
       <c r="C34" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D34" s="122" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34" s="122">
         <v>2</v>
       </c>
       <c r="F34" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" s="122">
         <v>1</v>
@@ -28853,17 +28767,17 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="122" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="122" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Halogen Incandescent, (1) 100W lampInterior CF 1L 23W Quad</v>
       </c>
       <c r="D35" s="123" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35" s="123">
         <v>1</v>
@@ -28874,17 +28788,17 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B36" s="122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="72" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Halogen Incandescent, (1) 35W lampPAR 20 Integral LED Lamp </v>
       </c>
       <c r="D36" s="123" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" s="123">
         <v>1</v>
@@ -28895,17 +28809,17 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="122" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Halogen Incandescent, (1) 50W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D37" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E37" s="122">
         <v>1</v>
@@ -28916,17 +28830,17 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="122" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Halogen Incandescent, (1) 60W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D38" s="123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E38" s="123">
         <v>1</v>
@@ -28937,17 +28851,17 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="122" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Halogen Incandescent, (1) 75W lampInterior CF 1L 23W Quad</v>
       </c>
       <c r="D39" s="123" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="123">
         <v>1</v>
@@ -28958,17 +28872,17 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B40" s="122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="72" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Halogen Incandescent, (1) 75W lampPAR 20 Integral LED Lamp </v>
       </c>
       <c r="D40" s="122" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E40" s="122">
         <v>1</v>
@@ -28979,17 +28893,17 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="122" t="s">
         <v>121</v>
-      </c>
-      <c r="B41" s="122" t="s">
-        <v>122</v>
       </c>
       <c r="C41" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Halogen, (1) Low Voltage MR16 lampMR 16 Integral LED Lamp</v>
       </c>
       <c r="D41" s="122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E41" s="122">
         <v>1</v>
@@ -29000,17 +28914,17 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B42" s="122" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 100W lampInterior CF 1L 23W Quad</v>
       </c>
       <c r="D42" s="122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E42" s="122">
         <v>1</v>
@@ -29021,17 +28935,17 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="122" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="72" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Incandescent, (1) 20W lampPAR 20 Integral LED Lamp </v>
       </c>
       <c r="D43" s="122" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E43" s="122">
         <v>1</v>
@@ -29042,17 +28956,17 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" s="122" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 25W lampMR 16 Integral LED Lamp</v>
       </c>
       <c r="D44" s="122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E44" s="122">
         <v>1</v>
@@ -29063,17 +28977,17 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B45" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 30W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D45" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" s="122">
         <v>1</v>
@@ -29084,17 +28998,17 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="122" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 40W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D46" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="122">
         <v>1</v>
@@ -29105,17 +29019,17 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="122" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B47" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 60W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D47" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E47" s="122">
         <v>1</v>
@@ -29126,17 +29040,17 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="122" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B48" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="72" t="str">
         <f>A48&amp;B48</f>
         <v>Incandescent, (1) 60W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D48" s="122" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E48" s="122">
         <v>1</v>
@@ -29144,22 +29058,22 @@
       <c r="F48" s="122"/>
       <c r="G48" s="122"/>
       <c r="H48" s="98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="122" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B49" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 65W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D49" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E49" s="122">
         <v>1</v>
@@ -29170,17 +29084,17 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="122" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 75W lampInterior CF 1L 13W Quad</v>
       </c>
       <c r="D50" s="122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E50" s="122">
         <v>1</v>
@@ -29191,17 +29105,17 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="122" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Incandescent, (1) 90W lampInterior CF 1L 23W Quad</v>
       </c>
       <c r="D51" s="122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E51" s="122">
         <v>1</v>
@@ -29212,17 +29126,17 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="122" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="122" t="s">
         <v>135</v>
-      </c>
-      <c r="B52" s="122" t="s">
-        <v>136</v>
       </c>
       <c r="C52" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Metal Halide, (1) 350W lamp, Magnetic ballastFluorescent, (4) 45.8", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)</v>
       </c>
       <c r="D52" s="122" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E52" s="122">
         <v>4</v>
@@ -29233,17 +29147,17 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="122" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B53" s="122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Metal Halide, (1) 400W lamp, Magnetic ballastFluorescent, (4) 45.8", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)</v>
       </c>
       <c r="D53" s="122" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" s="122">
         <v>4</v>
@@ -29270,7 +29184,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="C56" s="72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G56" s="98"/>
       <c r="H56" s="98"/>
@@ -29350,7 +29264,7 @@
       <c r="C75" s="72"/>
     </row>
     <row r="76" spans="2:3">
-      <c r="C76" s="133"/>
+      <c r="C76" s="132"/>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="72"/>
@@ -29365,260 +29279,354 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV34"/>
+  <dimension ref="A1:IV35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:D15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="98" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="98" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="98" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" style="98" customWidth="1"/>
-    <col min="5" max="256" width="9.109375" style="98" customWidth="1"/>
-    <col min="257" max="16384" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="13.85546875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="98" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="98" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="98" customWidth="1"/>
+    <col min="5" max="256" width="9.140625" style="98" customWidth="1"/>
+    <col min="257" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="87" customHeight="1">
       <c r="A1" s="124"/>
-      <c r="B1" s="186" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="187"/>
-      <c r="D1" s="188"/>
+      <c r="B1" s="184" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="185"/>
+      <c r="D1" s="186"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="169" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="171"/>
+      <c r="C2" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="184" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="185"/>
+      <c r="D2" s="183"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="183" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="185"/>
+      <c r="A3" s="178"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="181" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="183"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>50</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="125"/>
-      <c r="B5" s="189"/>
-      <c r="C5" s="190"/>
-      <c r="D5" s="191"/>
+      <c r="A5" s="125" t="str">
+        <f>IF('Audit Master'!L80=0, "", 'Audit Master'!L80)</f>
+        <v/>
+      </c>
+      <c r="B5" s="187" t="str">
+        <f>IF(A5="", "", "Philips 40820-3")</f>
+        <v/>
+      </c>
+      <c r="C5" s="188"/>
+      <c r="D5" s="189"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="126"/>
-      <c r="B6" s="177"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179"/>
+      <c r="A6" s="125" t="str">
+        <f>IF('Audit Master'!M80=0, "", 'Audit Master'!M80)</f>
+        <v/>
+      </c>
+      <c r="B6" s="187" t="str">
+        <f>IF(A6="", "", "TCP 20714")</f>
+        <v/>
+      </c>
+      <c r="C6" s="188"/>
+      <c r="D6" s="189"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="127"/>
-      <c r="B7" s="177"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="179"/>
+      <c r="A7" s="125" t="str">
+        <f>IF('Audit Master'!N80=0, "", 'Audit Master'!N80)</f>
+        <v/>
+      </c>
+      <c r="B7" s="187" t="str">
+        <f>IF(A7="", "", "Sylvania F017XP")</f>
+        <v/>
+      </c>
+      <c r="C7" s="188"/>
+      <c r="D7" s="189"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="126"/>
-      <c r="B8" s="177"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="179"/>
+      <c r="A8" s="126" t="str">
+        <f>IF('Audit Master'!O80=0, "", 'Audit Master'!O80)</f>
+        <v/>
+      </c>
+      <c r="B8" s="187" t="str">
+        <f>IF(A8="", "", "Sylvania F028SS")</f>
+        <v/>
+      </c>
+      <c r="C8" s="188"/>
+      <c r="D8" s="189"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="126"/>
-      <c r="B9" s="177"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="179"/>
+      <c r="A9" s="126" t="str">
+        <f>IF('Audit Master'!P80=0, "", 'Audit Master'!P80)</f>
+        <v/>
+      </c>
+      <c r="B9" s="187" t="str">
+        <f>IF(A9="", "", "Sylvania F032XP")</f>
+        <v/>
+      </c>
+      <c r="C9" s="188"/>
+      <c r="D9" s="189"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="126"/>
-      <c r="B10" s="177"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="179"/>
+      <c r="A10" s="126" t="str">
+        <f>IF('Audit Master'!Q80=0, "", 'Audit Master'!Q80)</f>
+        <v/>
+      </c>
+      <c r="B10" s="187" t="str">
+        <f>IF(A10="", "", "Sylvania FB030")</f>
+        <v/>
+      </c>
+      <c r="C10" s="188"/>
+      <c r="D10" s="189"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="126"/>
-      <c r="B11" s="177"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="179"/>
+      <c r="A11" s="126" t="str">
+        <f>IF('Audit Master'!R80=0, "", 'Audit Master'!R80)</f>
+        <v/>
+      </c>
+      <c r="B11" s="187" t="str">
+        <f>IF(A11="", "", "TCP 33123SP")</f>
+        <v/>
+      </c>
+      <c r="C11" s="188"/>
+      <c r="D11" s="189"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="126"/>
-      <c r="B12" s="177"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="179"/>
+      <c r="A12" s="126" t="str">
+        <f>IF('Audit Master'!S80=0, "", 'Audit Master'!S80)</f>
+        <v/>
+      </c>
+      <c r="B12" s="187" t="str">
+        <f>IF(A12="", "", "TCP 33113SP")</f>
+        <v/>
+      </c>
+      <c r="C12" s="188"/>
+      <c r="D12" s="189"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="126"/>
-      <c r="B13" s="177"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="179"/>
+      <c r="A13" s="126" t="str">
+        <f>IF('Audit Master'!T80=0, "", 'Audit Master'!T80)</f>
+        <v/>
+      </c>
+      <c r="B13" s="187" t="str">
+        <f>IF(A13="", "", "Philips 40877-3")</f>
+        <v/>
+      </c>
+      <c r="C13" s="188"/>
+      <c r="D13" s="189"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="126"/>
-      <c r="B14" s="177"/>
-      <c r="C14" s="178"/>
-      <c r="D14" s="179"/>
+      <c r="A14" s="126" t="str">
+        <f>IF('Audit Master'!U80=0, "", 'Audit Master'!U80)</f>
+        <v/>
+      </c>
+      <c r="B14" s="187" t="str">
+        <f>IF(A14="", "", "TCP 33213SSP")</f>
+        <v/>
+      </c>
+      <c r="C14" s="188"/>
+      <c r="D14" s="189"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="126"/>
-      <c r="B15" s="177"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="179"/>
+      <c r="A15" s="126" t="str">
+        <f>IF('Audit Master'!V80=0, "", 'Audit Master'!V80)</f>
+        <v/>
+      </c>
+      <c r="B15" s="187" t="str">
+        <f>IF(A15="", "", "Sylvania FP54T5HO")</f>
+        <v/>
+      </c>
+      <c r="C15" s="188"/>
+      <c r="D15" s="189"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="128"/>
-      <c r="B16" s="180"/>
-      <c r="C16" s="181"/>
-      <c r="D16" s="182"/>
+      <c r="A16" s="127" t="str">
+        <f>IF('Audit Master'!W80=0, "", 'Audit Master'!W80)</f>
+        <v/>
+      </c>
+      <c r="B16" s="187" t="str">
+        <f>IF(A16="", "", "Sylvania QHE2X32T8/UNV ISL-SC")</f>
+        <v/>
+      </c>
+      <c r="C16" s="188"/>
+      <c r="D16" s="189"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="128"/>
-      <c r="B17" s="180"/>
-      <c r="C17" s="181"/>
-      <c r="D17" s="182"/>
+      <c r="A17" s="126" t="str">
+        <f>IF('Audit Master'!X80=0, "", 'Audit Master'!X80)</f>
+        <v/>
+      </c>
+      <c r="B17" s="187" t="str">
+        <f>IF(A17="", "", "Sylvania QHE4X32T8/UNV ISL-SC")</f>
+        <v/>
+      </c>
+      <c r="C17" s="188"/>
+      <c r="D17" s="189"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="129"/>
-      <c r="B18" s="180"/>
-      <c r="C18" s="181"/>
-      <c r="D18" s="182"/>
+      <c r="A18" s="126" t="str">
+        <f>IF('Audit Master'!Y80=0, "", 'Audit Master'!Y80)</f>
+        <v/>
+      </c>
+      <c r="B18" s="187" t="str">
+        <f>IF(A18="", "", "Sylvania QHE4X32T8/UNV ISN-SC")</f>
+        <v/>
+      </c>
+      <c r="C18" s="188"/>
+      <c r="D18" s="189"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="183"/>
-      <c r="B19" s="184"/>
-      <c r="C19" s="184"/>
-      <c r="D19" s="185"/>
+      <c r="A19" s="128" t="str">
+        <f>IF('Audit Master'!Z80=0, "", 'Audit Master'!Z80)</f>
+        <v/>
+      </c>
+      <c r="B19" s="187" t="str">
+        <f>IF(A19="", "", "Sylvania QHE4X32T8/UNV ISH")</f>
+        <v/>
+      </c>
+      <c r="C19" s="188"/>
+      <c r="D19" s="189"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="171" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
+      <c r="A20" s="181"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="183"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="160"/>
-      <c r="B21" s="161"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
+      <c r="A21" s="175" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="176"/>
+      <c r="C21" s="176"/>
+      <c r="D21" s="177"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="160"/>
-      <c r="B22" s="161"/>
-      <c r="C22" s="161"/>
-      <c r="D22" s="162"/>
+      <c r="A22" s="164"/>
+      <c r="B22" s="165"/>
+      <c r="C22" s="165"/>
+      <c r="D22" s="166"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="168"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="169"/>
-      <c r="D23" s="170"/>
+      <c r="A23" s="164"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="166"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="165" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="166"/>
-      <c r="C24" s="166"/>
-      <c r="D24" s="167"/>
+      <c r="A24" s="172"/>
+      <c r="B24" s="173"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="174"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="168"/>
-      <c r="B25" s="169"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="170"/>
+      <c r="A25" s="169" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="170"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="171"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="165" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="167"/>
+      <c r="A26" s="172"/>
+      <c r="B26" s="173"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="174"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="171"/>
-      <c r="B27" s="172"/>
-      <c r="C27" s="172"/>
-      <c r="D27" s="173"/>
+      <c r="A27" s="169" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="170"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="171"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="174"/>
-      <c r="B28" s="175"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="176"/>
+      <c r="A28" s="175"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="177"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="165" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="166"/>
-      <c r="C29" s="166"/>
-      <c r="D29" s="167"/>
+      <c r="A29" s="178"/>
+      <c r="B29" s="179"/>
+      <c r="C29" s="179"/>
+      <c r="D29" s="180"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="160"/>
-      <c r="B30" s="161"/>
-      <c r="C30" s="161"/>
-      <c r="D30" s="162"/>
+      <c r="A30" s="169" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="170"/>
+      <c r="C30" s="170"/>
+      <c r="D30" s="171"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A31" s="160"/>
-      <c r="B31" s="161"/>
-      <c r="C31" s="161"/>
-      <c r="D31" s="162"/>
+    <row r="31" spans="1:4">
+      <c r="A31" s="164"/>
+      <c r="B31" s="165"/>
+      <c r="C31" s="165"/>
+      <c r="D31" s="166"/>
     </row>
-    <row r="32" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A32" s="163" t="s">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="164"/>
+      <c r="B32" s="165"/>
+      <c r="C32" s="165"/>
+      <c r="D32" s="166"/>
+    </row>
+    <row r="33" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A33" s="167" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="168"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="164"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="21" customHeight="1" thickBot="1">
+      <c r="A34" s="23" t="s">
         <v>56</v>
       </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="24"/>
     </row>
-    <row r="33" spans="1:4" ht="21" customHeight="1" thickBot="1">
-      <c r="A33" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25" t="s">
+    <row r="35" spans="1:4" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A35" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="24"/>
-    </row>
-    <row r="34" spans="1:4" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A34" s="23" t="s">
+      <c r="B35" s="129"/>
+      <c r="C35" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="130"/>
-      <c r="C34" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="130"/>
+      <c r="D35" s="129"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A2:B2"/>
@@ -29631,27 +29639,28 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added changes, now for testing
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ala\Documents\GitHub\MatrixPepco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaar_000\Documents\GitHub\MatrixPepco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8184"/>
   </bookViews>
   <sheets>
     <sheet name="Audit Master" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="143">
   <si>
     <t>Business Name:</t>
   </si>
@@ -549,6 +549,15 @@
   <si>
     <t>Phone Number:</t>
   </si>
+  <si>
+    <t>Fluorescent, (3) 48", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
+  </si>
+  <si>
+    <t>Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
+  </si>
+  <si>
+    <t>Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
+  </si>
 </sst>
 </file>
 
@@ -568,7 +577,7 @@
     <numFmt numFmtId="170" formatCode="_(#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="171" formatCode="_(#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="69">
+  <fonts count="70">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -989,6 +998,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -4026,7 +4042,7 @@
     <xf numFmtId="3" fontId="44" fillId="0" borderId="18" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4342,6 +4358,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="49" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4372,67 +4424,46 @@
     <xf numFmtId="0" fontId="60" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4453,42 +4484,31 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2059">
     <cellStyle name="20% - Accent1 2" xfId="33"/>
@@ -22208,28 +22228,26 @@
   </sheetPr>
   <dimension ref="A1:IM93"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" style="39" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="36.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="1" customWidth="1"/>
-    <col min="13" max="25" width="9.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" style="1" customWidth="1"/>
-    <col min="27" max="247" width="9.140625" style="1" customWidth="1"/>
-    <col min="248" max="16384" width="8.85546875" style="26"/>
+    <col min="1" max="1" width="5.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="41" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="36.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" style="1" customWidth="1"/>
+    <col min="13" max="25" width="9.109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" style="1" customWidth="1"/>
+    <col min="27" max="247" width="9.109375" style="1" customWidth="1"/>
+    <col min="248" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="21.6" customHeight="1">
@@ -22259,7 +22277,7 @@
       </c>
       <c r="L2" s="29"/>
     </row>
-    <row r="3" spans="1:27" ht="19.149999999999999" customHeight="1">
+    <row r="3" spans="1:27" ht="19.2" customHeight="1">
       <c r="A3" s="37" t="s">
         <v>15</v>
       </c>
@@ -22281,15 +22299,15 @@
       <c r="K4" s="6"/>
       <c r="R4" s="130"/>
     </row>
-    <row r="5" spans="1:27" ht="24.4" customHeight="1">
-      <c r="A5" s="158" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="159"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
+    <row r="5" spans="1:27" ht="24.45" customHeight="1">
+      <c r="A5" s="147" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="148"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
       <c r="G5" s="44" t="s">
         <v>139</v>
       </c>
@@ -22300,15 +22318,15 @@
       <c r="L5" s="47"/>
       <c r="R5" s="135"/>
     </row>
-    <row r="6" spans="1:27" ht="24.4" customHeight="1">
-      <c r="A6" s="158" t="s">
+    <row r="6" spans="1:27" ht="24.45" customHeight="1">
+      <c r="A6" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="149"/>
+      <c r="B6" s="148"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
       <c r="G6" s="44"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
@@ -22317,17 +22335,17 @@
       <c r="L6" s="47"/>
       <c r="R6" s="135"/>
     </row>
-    <row r="7" spans="1:27" ht="24.4" customHeight="1">
-      <c r="A7" s="158" t="s">
+    <row r="7" spans="1:27" ht="24.45" customHeight="1">
+      <c r="A7" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="159"/>
-      <c r="C7" s="149" t="s">
+      <c r="B7" s="148"/>
+      <c r="C7" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="149"/>
-      <c r="E7" s="149"/>
-      <c r="F7" s="149"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
       <c r="G7" s="44" t="s">
         <v>39</v>
       </c>
@@ -22339,17 +22357,17 @@
       <c r="R7" s="135"/>
       <c r="AA7" s="130"/>
     </row>
-    <row r="8" spans="1:27" ht="24.4" customHeight="1">
-      <c r="A8" s="158" t="s">
+    <row r="8" spans="1:27" ht="24.45" customHeight="1">
+      <c r="A8" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="150" t="s">
+      <c r="B8" s="148"/>
+      <c r="C8" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="150"/>
-      <c r="E8" s="150"/>
-      <c r="F8" s="150"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
       <c r="G8" s="51" t="s">
         <v>43</v>
       </c>
@@ -22361,7 +22379,7 @@
       <c r="R8" s="130"/>
       <c r="AA8" s="130"/>
     </row>
-    <row r="9" spans="1:27" ht="24.4" hidden="1" customHeight="1">
+    <row r="9" spans="1:27" ht="24.45" hidden="1" customHeight="1">
       <c r="A9" s="136"/>
       <c r="B9" s="137"/>
       <c r="C9" s="138"/>
@@ -22377,7 +22395,7 @@
       <c r="R9" s="130"/>
       <c r="AA9" s="130"/>
     </row>
-    <row r="10" spans="1:27" ht="24.4" customHeight="1">
+    <row r="10" spans="1:27" ht="24.45" customHeight="1">
       <c r="A10" s="52"/>
       <c r="B10" s="53"/>
       <c r="C10" s="53"/>
@@ -22390,7 +22408,7 @@
       <c r="R10" s="130"/>
       <c r="AA10" s="130"/>
     </row>
-    <row r="11" spans="1:27" ht="10.15" customHeight="1" thickBot="1">
+    <row r="11" spans="1:27" ht="10.199999999999999" customHeight="1" thickBot="1">
       <c r="A11" s="56"/>
       <c r="B11" s="38"/>
       <c r="D11" s="57"/>
@@ -22408,18 +22426,18 @@
         <v>4</v>
       </c>
       <c r="E12" s="61"/>
-      <c r="F12" s="151" t="s">
+      <c r="F12" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="155"/>
-      <c r="H12" s="155"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
       <c r="I12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="151" t="s">
+      <c r="J12" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="152"/>
+      <c r="K12" s="163"/>
       <c r="L12" s="63"/>
       <c r="AA12" s="130"/>
     </row>
@@ -22502,7 +22520,7 @@
       </c>
       <c r="AA13" s="130"/>
     </row>
-    <row r="14" spans="1:27" ht="29.45" customHeight="1">
+    <row r="14" spans="1:27" ht="29.4" customHeight="1">
       <c r="A14" s="74">
         <v>1</v>
       </c>
@@ -22568,12 +22586,12 @@
         <v>0</v>
       </c>
       <c r="X14" s="1">
-        <f>IF(OR(D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D14&amp;F14="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G14*1,
+        <f>IF(OR(D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D14&amp;F14="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G14*1,
 IF(D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", G14*2, 0))</f>
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <f>IF(OR(D14&amp;F14="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G14*1,
+        <f>IF(OR(D14&amp;F14="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G14*1,
 IF(D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", G14*2, 0))</f>
         <v>0</v>
       </c>
@@ -22583,7 +22601,7 @@
       </c>
       <c r="AA14" s="130"/>
     </row>
-    <row r="15" spans="1:27" ht="29.45" customHeight="1">
+    <row r="15" spans="1:27" ht="29.4" customHeight="1">
       <c r="A15" s="74">
         <v>2</v>
       </c>
@@ -22649,12 +22667,12 @@
         <v>0</v>
       </c>
       <c r="X15" s="1">
-        <f t="shared" ref="X15:X78" si="12">IF(OR(D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D15&amp;F15="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G15*1,
+        <f t="shared" ref="X15:X78" si="12">IF(OR(D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D15&amp;F15="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G15*1,
 IF(D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", G15*2, 0))</f>
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <f t="shared" ref="Y15:Y78" si="13">IF(OR(D15&amp;F15="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G15*1,
+        <f t="shared" ref="Y15:Y78" si="13">IF(OR(D15&amp;F15="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G15*1,
 IF(D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", G15*2, 0))</f>
         <v>0</v>
       </c>
@@ -22664,7 +22682,7 @@
       </c>
       <c r="AA15" s="130"/>
     </row>
-    <row r="16" spans="1:27" ht="29.45" customHeight="1">
+    <row r="16" spans="1:27" ht="29.4" customHeight="1">
       <c r="A16" s="74">
         <v>3</v>
       </c>
@@ -22740,7 +22758,7 @@
       </c>
       <c r="AA16" s="130"/>
     </row>
-    <row r="17" spans="1:27" ht="29.45" customHeight="1">
+    <row r="17" spans="1:27" ht="29.4" customHeight="1">
       <c r="A17" s="74">
         <v>4</v>
       </c>
@@ -22816,7 +22834,7 @@
       </c>
       <c r="AA17" s="130"/>
     </row>
-    <row r="18" spans="1:27" ht="29.45" customHeight="1">
+    <row r="18" spans="1:27" ht="29.4" customHeight="1">
       <c r="A18" s="74">
         <v>5</v>
       </c>
@@ -22892,7 +22910,7 @@
       </c>
       <c r="AA18" s="130"/>
     </row>
-    <row r="19" spans="1:27" ht="29.45" customHeight="1">
+    <row r="19" spans="1:27" ht="29.4" customHeight="1">
       <c r="A19" s="74">
         <v>6</v>
       </c>
@@ -22968,7 +22986,7 @@
       </c>
       <c r="AA19" s="130"/>
     </row>
-    <row r="20" spans="1:27" ht="29.45" customHeight="1">
+    <row r="20" spans="1:27" ht="29.4" customHeight="1">
       <c r="A20" s="74">
         <v>7</v>
       </c>
@@ -23044,7 +23062,7 @@
       </c>
       <c r="AA20" s="130"/>
     </row>
-    <row r="21" spans="1:27" ht="29.45" customHeight="1">
+    <row r="21" spans="1:27" ht="29.4" customHeight="1">
       <c r="A21" s="74">
         <v>8</v>
       </c>
@@ -23120,7 +23138,7 @@
       </c>
       <c r="AA21" s="130"/>
     </row>
-    <row r="22" spans="1:27" ht="29.45" customHeight="1">
+    <row r="22" spans="1:27" ht="29.4" customHeight="1">
       <c r="A22" s="74">
         <v>9</v>
       </c>
@@ -23196,7 +23214,7 @@
       </c>
       <c r="AA22" s="130"/>
     </row>
-    <row r="23" spans="1:27" ht="29.45" customHeight="1">
+    <row r="23" spans="1:27" ht="29.4" customHeight="1">
       <c r="A23" s="74">
         <v>10</v>
       </c>
@@ -23271,7 +23289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="29.45" customHeight="1">
+    <row r="24" spans="1:27" ht="29.4" customHeight="1">
       <c r="A24" s="74">
         <v>11</v>
       </c>
@@ -23346,7 +23364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="29.45" customHeight="1">
+    <row r="25" spans="1:27" ht="29.4" customHeight="1">
       <c r="A25" s="74">
         <v>12</v>
       </c>
@@ -23421,7 +23439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="29.45" customHeight="1" thickBot="1">
+    <row r="26" spans="1:27" ht="29.4" customHeight="1">
       <c r="A26" s="74">
         <v>13</v>
       </c>
@@ -23496,7 +23514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="27" spans="1:27" ht="29.4" customHeight="1">
       <c r="A27" s="74">
         <v>14</v>
       </c>
@@ -23571,7 +23589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="28" spans="1:27" ht="29.4" customHeight="1">
       <c r="A28" s="74">
         <v>15</v>
       </c>
@@ -23646,7 +23664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="29" spans="1:27" ht="29.4" customHeight="1">
       <c r="A29" s="74">
         <v>16</v>
       </c>
@@ -23721,7 +23739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="30" spans="1:27" ht="29.4" customHeight="1">
       <c r="A30" s="74">
         <v>17</v>
       </c>
@@ -23796,7 +23814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="31" spans="1:27" ht="29.4" customHeight="1">
       <c r="A31" s="74">
         <v>18</v>
       </c>
@@ -23871,7 +23889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="32" spans="1:27" ht="29.4" customHeight="1">
       <c r="A32" s="74">
         <v>19</v>
       </c>
@@ -23946,7 +23964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="33" spans="1:26" ht="29.4" customHeight="1">
       <c r="A33" s="74">
         <v>20</v>
       </c>
@@ -24021,7 +24039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="34" spans="1:26" ht="29.4" customHeight="1">
       <c r="A34" s="74">
         <v>21</v>
       </c>
@@ -24096,7 +24114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="35" spans="1:26" ht="29.4" customHeight="1">
       <c r="A35" s="74">
         <v>22</v>
       </c>
@@ -24171,7 +24189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="36" spans="1:26" ht="29.4" customHeight="1">
       <c r="A36" s="74">
         <v>23</v>
       </c>
@@ -24246,7 +24264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="37" spans="1:26" ht="29.4" customHeight="1">
       <c r="A37" s="74">
         <v>24</v>
       </c>
@@ -24321,7 +24339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="38" spans="1:26" ht="29.4" customHeight="1">
       <c r="A38" s="74">
         <v>25</v>
       </c>
@@ -24396,7 +24414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="39" spans="1:26" ht="29.4" customHeight="1">
       <c r="A39" s="74">
         <v>26</v>
       </c>
@@ -24471,7 +24489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="40" spans="1:26" ht="29.4" customHeight="1">
       <c r="A40" s="74">
         <v>27</v>
       </c>
@@ -24546,7 +24564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="41" spans="1:26" ht="29.4" customHeight="1">
       <c r="A41" s="74">
         <v>28</v>
       </c>
@@ -24621,7 +24639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="42" spans="1:26" ht="29.4" customHeight="1">
       <c r="A42" s="74">
         <v>29</v>
       </c>
@@ -24696,7 +24714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="43" spans="1:26" ht="29.4" customHeight="1">
       <c r="A43" s="74">
         <v>30</v>
       </c>
@@ -24771,7 +24789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="44" spans="1:26" ht="29.4" customHeight="1">
       <c r="A44" s="74">
         <v>31</v>
       </c>
@@ -24846,7 +24864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="45" spans="1:26" ht="29.4" customHeight="1">
       <c r="A45" s="74">
         <v>32</v>
       </c>
@@ -24921,7 +24939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="46" spans="1:26" ht="29.4" customHeight="1">
       <c r="A46" s="74">
         <v>33</v>
       </c>
@@ -24996,7 +25014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="47" spans="1:26" ht="29.4" customHeight="1">
       <c r="A47" s="74">
         <v>34</v>
       </c>
@@ -25071,7 +25089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="48" spans="1:26" ht="29.4" customHeight="1">
       <c r="A48" s="74">
         <v>35</v>
       </c>
@@ -25146,7 +25164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="49" spans="1:27" ht="29.4" customHeight="1">
       <c r="A49" s="74">
         <v>36</v>
       </c>
@@ -25221,7 +25239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="50" spans="1:27" ht="29.4" customHeight="1">
       <c r="A50" s="74">
         <v>37</v>
       </c>
@@ -25296,7 +25314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="51" spans="1:27" ht="29.4" customHeight="1">
       <c r="A51" s="74">
         <v>38</v>
       </c>
@@ -25372,7 +25390,7 @@
       </c>
       <c r="AA51" s="130"/>
     </row>
-    <row r="52" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="52" spans="1:27" ht="29.4" customHeight="1">
       <c r="A52" s="74">
         <v>39</v>
       </c>
@@ -25447,7 +25465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="53" spans="1:27" ht="29.4" customHeight="1">
       <c r="A53" s="74">
         <v>40</v>
       </c>
@@ -25522,7 +25540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="54" spans="1:27" ht="29.4" customHeight="1">
       <c r="A54" s="74">
         <v>41</v>
       </c>
@@ -25597,7 +25615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="55" spans="1:27" ht="29.4" customHeight="1">
       <c r="A55" s="74">
         <v>42</v>
       </c>
@@ -25672,7 +25690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="56" spans="1:27" ht="29.4" customHeight="1">
       <c r="A56" s="74">
         <v>43</v>
       </c>
@@ -25747,7 +25765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="57" spans="1:27" ht="29.4" customHeight="1">
       <c r="A57" s="74">
         <v>44</v>
       </c>
@@ -25822,7 +25840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="58" spans="1:27" ht="29.4" customHeight="1">
       <c r="A58" s="74">
         <v>45</v>
       </c>
@@ -25897,7 +25915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="59" spans="1:27" ht="29.4" customHeight="1">
       <c r="A59" s="74">
         <v>46</v>
       </c>
@@ -25972,7 +25990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="60" spans="1:27" ht="29.4" customHeight="1">
       <c r="A60" s="74">
         <v>47</v>
       </c>
@@ -26047,7 +26065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="61" spans="1:27" ht="29.4" customHeight="1">
       <c r="A61" s="74">
         <v>48</v>
       </c>
@@ -26122,7 +26140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="62" spans="1:27" ht="29.4" customHeight="1">
       <c r="A62" s="74">
         <v>49</v>
       </c>
@@ -26197,7 +26215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="63" spans="1:27" ht="29.4" customHeight="1">
       <c r="A63" s="74">
         <v>50</v>
       </c>
@@ -26272,7 +26290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="29.45" hidden="1" customHeight="1">
+    <row r="64" spans="1:27" ht="29.4" customHeight="1">
       <c r="A64" s="74">
         <v>51</v>
       </c>
@@ -26347,7 +26365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="65" spans="1:26" ht="29.4" customHeight="1">
       <c r="A65" s="74">
         <v>52</v>
       </c>
@@ -26422,7 +26440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="66" spans="1:26" ht="29.4" customHeight="1">
       <c r="A66" s="74">
         <v>53</v>
       </c>
@@ -26497,7 +26515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="67" spans="1:26" ht="29.4" customHeight="1">
       <c r="A67" s="74">
         <v>54</v>
       </c>
@@ -26572,7 +26590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="68" spans="1:26" ht="29.4" customHeight="1">
       <c r="A68" s="74">
         <v>55</v>
       </c>
@@ -26647,7 +26665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="69" spans="1:26" ht="29.4" customHeight="1">
       <c r="A69" s="74">
         <v>56</v>
       </c>
@@ -26722,7 +26740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="70" spans="1:26" ht="29.4" customHeight="1">
       <c r="A70" s="74">
         <v>57</v>
       </c>
@@ -26797,7 +26815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="71" spans="1:26" ht="29.4" customHeight="1">
       <c r="A71" s="74">
         <v>58</v>
       </c>
@@ -26872,7 +26890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="72" spans="1:26" ht="29.4" customHeight="1">
       <c r="A72" s="74">
         <v>59</v>
       </c>
@@ -26947,7 +26965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="73" spans="1:26" ht="29.4" customHeight="1">
       <c r="A73" s="74">
         <v>60</v>
       </c>
@@ -27022,7 +27040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="74" spans="1:26" ht="29.4" customHeight="1">
       <c r="A74" s="74">
         <v>61</v>
       </c>
@@ -27097,7 +27115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="75" spans="1:26" ht="29.4" customHeight="1">
       <c r="A75" s="74">
         <v>62</v>
       </c>
@@ -27172,7 +27190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="76" spans="1:26" ht="29.4" customHeight="1">
       <c r="A76" s="74">
         <v>63</v>
       </c>
@@ -27247,7 +27265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="77" spans="1:26" ht="29.4" customHeight="1">
       <c r="A77" s="74">
         <v>64</v>
       </c>
@@ -27322,7 +27340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="29.45" hidden="1" customHeight="1">
+    <row r="78" spans="1:26" ht="29.4" customHeight="1">
       <c r="A78" s="74">
         <v>65</v>
       </c>
@@ -27397,7 +27415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="29.45" hidden="1" customHeight="1" thickBot="1">
+    <row r="79" spans="1:26" ht="29.4" customHeight="1" thickBot="1">
       <c r="A79" s="74">
         <v>66</v>
       </c>
@@ -27463,12 +27481,12 @@
         <v>0</v>
       </c>
       <c r="X79" s="1">
-        <f t="shared" ref="X79" si="27">IF(OR(D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1,
+        <f t="shared" ref="X79" si="27">IF(OR(D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1,
 IF(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", G79*2, 0))</f>
         <v>0</v>
       </c>
       <c r="Y79" s="1">
-        <f t="shared" ref="Y79" si="28">IF(OR(D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1,
+        <f t="shared" ref="Y79" si="28">IF(OR(D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1,
 IF(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", G79*2, 0))</f>
         <v>0</v>
       </c>
@@ -27477,7 +27495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="19.149999999999999" customHeight="1" thickTop="1">
+    <row r="80" spans="1:26" ht="19.2" customHeight="1" thickTop="1">
       <c r="A80" s="93"/>
       <c r="B80" s="94" t="s">
         <v>17</v>
@@ -27553,7 +27571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="19.149999999999999" customHeight="1">
+    <row r="81" spans="1:12" ht="19.2" customHeight="1">
       <c r="A81" s="93"/>
       <c r="B81" s="96"/>
       <c r="C81" s="94" t="s">
@@ -27568,7 +27586,7 @@
       <c r="I81" s="94"/>
       <c r="K81" s="6"/>
     </row>
-    <row r="82" spans="1:12" ht="19.149999999999999" customHeight="1">
+    <row r="82" spans="1:12" ht="19.2" customHeight="1">
       <c r="A82" s="93"/>
       <c r="B82" s="96"/>
       <c r="C82" s="94" t="s">
@@ -27583,7 +27601,7 @@
       <c r="I82" s="94"/>
       <c r="K82" s="6"/>
     </row>
-    <row r="83" spans="1:12" ht="19.149999999999999" customHeight="1">
+    <row r="83" spans="1:12" ht="19.2" customHeight="1">
       <c r="A83" s="93"/>
       <c r="B83" s="96"/>
       <c r="D83" s="94"/>
@@ -27595,30 +27613,30 @@
       <c r="I83" s="94"/>
       <c r="K83" s="6"/>
     </row>
-    <row r="84" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1" thickBot="1">
-      <c r="A84" s="162"/>
-      <c r="B84" s="163"/>
+    <row r="84" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
+      <c r="A84" s="151"/>
+      <c r="B84" s="152"/>
       <c r="C84" s="97"/>
       <c r="D84" s="97"/>
       <c r="E84" s="97"/>
-      <c r="F84" s="163"/>
-      <c r="G84" s="163"/>
+      <c r="F84" s="152"/>
+      <c r="G84" s="152"/>
       <c r="H84" s="97"/>
       <c r="I84" s="97"/>
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A85" s="153" t="s">
+      <c r="A85" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="154"/>
+      <c r="B85" s="142"/>
       <c r="C85" s="100"/>
       <c r="D85" s="100"/>
       <c r="E85" s="100"/>
-      <c r="F85" s="154" t="s">
+      <c r="F85" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="154"/>
+      <c r="G85" s="142"/>
       <c r="J85" s="7" t="s">
         <v>35</v>
       </c>
@@ -27633,10 +27651,10 @@
       <c r="E86" s="102"/>
       <c r="F86" s="102"/>
       <c r="G86" s="102"/>
-      <c r="J86" s="141" t="s">
+      <c r="J86" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="K86" s="142"/>
+      <c r="K86" s="154"/>
       <c r="L86" s="30"/>
     </row>
     <row r="87" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
@@ -27647,43 +27665,43 @@
       <c r="E87" s="102"/>
       <c r="F87" s="102"/>
       <c r="G87" s="102"/>
-      <c r="J87" s="143"/>
-      <c r="K87" s="144"/>
+      <c r="J87" s="155"/>
+      <c r="K87" s="156"/>
       <c r="L87" s="30"/>
     </row>
-    <row r="88" spans="1:12" s="98" customFormat="1" ht="22.9" customHeight="1" thickBot="1">
-      <c r="A88" s="160"/>
-      <c r="B88" s="161"/>
+    <row r="88" spans="1:12" s="98" customFormat="1" ht="22.95" customHeight="1" thickBot="1">
+      <c r="A88" s="149"/>
+      <c r="B88" s="150"/>
       <c r="C88" s="103"/>
       <c r="D88" s="103"/>
       <c r="E88" s="103"/>
-      <c r="F88" s="161"/>
-      <c r="G88" s="161"/>
+      <c r="F88" s="150"/>
+      <c r="G88" s="150"/>
       <c r="H88" s="97"/>
       <c r="I88" s="97"/>
-      <c r="J88" s="145" t="s">
+      <c r="J88" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="K88" s="146"/>
+      <c r="K88" s="158"/>
       <c r="L88" s="104"/>
     </row>
-    <row r="89" spans="1:12" s="98" customFormat="1" ht="17.45" customHeight="1">
-      <c r="A89" s="153" t="s">
+    <row r="89" spans="1:12" s="98" customFormat="1" ht="17.399999999999999" customHeight="1">
+      <c r="A89" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="154"/>
+      <c r="B89" s="142"/>
       <c r="C89" s="100"/>
       <c r="D89" s="100"/>
       <c r="E89" s="100"/>
-      <c r="F89" s="154" t="s">
+      <c r="F89" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="G89" s="154"/>
-      <c r="J89" s="147"/>
-      <c r="K89" s="148"/>
+      <c r="G89" s="142"/>
+      <c r="J89" s="159"/>
+      <c r="K89" s="160"/>
       <c r="L89" s="104"/>
     </row>
-    <row r="90" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1">
+    <row r="90" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1">
       <c r="A90" s="101"/>
       <c r="B90" s="102"/>
       <c r="C90" s="102"/>
@@ -27713,18 +27731,18 @@
       <c r="K91" s="109"/>
       <c r="L91" s="110"/>
     </row>
-    <row r="92" spans="1:12" s="98" customFormat="1" ht="25.15" customHeight="1" thickBot="1">
-      <c r="A92" s="156" t="s">
+    <row r="92" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
+      <c r="A92" s="145" t="s">
         <v>13</v>
       </c>
-      <c r="B92" s="157"/>
+      <c r="B92" s="146"/>
       <c r="C92" s="111"/>
       <c r="D92" s="111"/>
       <c r="E92" s="111"/>
-      <c r="F92" s="157" t="s">
+      <c r="F92" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="G92" s="157"/>
+      <c r="G92" s="146"/>
       <c r="H92" s="112"/>
       <c r="I92" s="113"/>
       <c r="J92" s="114" t="s">
@@ -27748,6 +27766,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J86:K87"/>
+    <mergeCell ref="J88:K89"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A92:B92"/>
@@ -27763,40 +27788,34 @@
     <mergeCell ref="F89:G89"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="F84:G84"/>
-    <mergeCell ref="J86:K87"/>
-    <mergeCell ref="J88:K89"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup scale="21" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="67.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92" style="98" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" style="98" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="98" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="98" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" style="98" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="26"/>
+    <col min="1" max="1" width="67.109375" style="98" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.88671875" style="98" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" style="98" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="98" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="98" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" style="98" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" customHeight="1">
@@ -27833,7 +27852,7 @@
       <c r="P1" s="27"/>
       <c r="Q1" s="27"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" hidden="1">
       <c r="A2" s="122" t="s">
         <v>66</v>
       </c>
@@ -27854,7 +27873,7 @@
       <c r="G2" s="122"/>
       <c r="H2" s="98"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" hidden="1">
       <c r="A3" s="122" t="s">
         <v>69</v>
       </c>
@@ -27875,7 +27894,7 @@
       <c r="G3" s="122"/>
       <c r="H3" s="98"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" hidden="1">
       <c r="A4" s="122" t="s">
         <v>70</v>
       </c>
@@ -27896,7 +27915,7 @@
       <c r="G4" s="122"/>
       <c r="H4" s="98"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" hidden="1">
       <c r="A5" s="122" t="s">
         <v>73</v>
       </c>
@@ -27917,7 +27936,7 @@
       <c r="G5" s="122"/>
       <c r="H5" s="98"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" hidden="1">
       <c r="A6" s="122" t="s">
         <v>75</v>
       </c>
@@ -27945,7 +27964,7 @@
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" hidden="1">
       <c r="A7" s="122" t="s">
         <v>79</v>
       </c>
@@ -28242,7 +28261,7 @@
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" hidden="1">
       <c r="A16" s="122" t="s">
         <v>93</v>
       </c>
@@ -28275,7 +28294,7 @@
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:19" hidden="1">
       <c r="A17" s="122" t="s">
         <v>93</v>
       </c>
@@ -28300,7 +28319,7 @@
       </c>
       <c r="H17" s="98"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:19" hidden="1">
       <c r="A18" s="122" t="s">
         <v>98</v>
       </c>
@@ -28325,7 +28344,7 @@
       </c>
       <c r="H18" s="98"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:19" hidden="1">
       <c r="A19" s="122" t="s">
         <v>99</v>
       </c>
@@ -28358,7 +28377,7 @@
       <c r="P19" s="27"/>
       <c r="Q19" s="27"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:19" hidden="1">
       <c r="A20" s="122" t="s">
         <v>100</v>
       </c>
@@ -28391,7 +28410,7 @@
       <c r="P20" s="98"/>
       <c r="Q20" s="27"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:19">
       <c r="A21" s="122" t="s">
         <v>101</v>
       </c>
@@ -28424,7 +28443,7 @@
       <c r="P21" s="27"/>
       <c r="Q21" s="27"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:19">
       <c r="A22" s="122" t="s">
         <v>102</v>
       </c>
@@ -28457,7 +28476,7 @@
       <c r="P22" s="27"/>
       <c r="Q22" s="27"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:19">
       <c r="A23" s="122" t="s">
         <v>103</v>
       </c>
@@ -28490,7 +28509,7 @@
       <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:19">
       <c r="A24" s="123" t="s">
         <v>104</v>
       </c>
@@ -28514,8 +28533,18 @@
         <v>1</v>
       </c>
       <c r="H24" s="98"/>
+      <c r="Q24" s="192" t="s">
+        <v>104</v>
+      </c>
+      <c r="R24" s="193" t="s">
+        <v>142</v>
+      </c>
+      <c r="S24" s="26" t="str">
+        <f>Q24&amp;R24</f>
+        <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
+      </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:19">
       <c r="A25" s="122" t="s">
         <v>105</v>
       </c>
@@ -28540,16 +28569,16 @@
       </c>
       <c r="H25" s="98"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:19">
       <c r="A26" s="123" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="122" t="s">
-        <v>89</v>
+      <c r="B26" s="190" t="s">
+        <v>140</v>
       </c>
       <c r="C26" s="72" t="str">
         <f t="shared" si="0"/>
-        <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)</v>
+        <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
       </c>
       <c r="D26" s="123" t="s">
         <v>81</v>
@@ -28557,15 +28586,18 @@
       <c r="E26" s="123">
         <v>4</v>
       </c>
-      <c r="F26" s="123" t="s">
-        <v>87</v>
+      <c r="F26" s="191" t="s">
+        <v>84</v>
       </c>
       <c r="G26" s="122">
         <v>1</v>
       </c>
       <c r="H26" s="98"/>
+      <c r="R26" s="26" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:19">
       <c r="A27" s="122" t="s">
         <v>105</v>
       </c>
@@ -28589,8 +28621,11 @@
         <v>1</v>
       </c>
       <c r="H27" s="98"/>
+      <c r="R27" s="26" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:19">
       <c r="A28" s="123" t="s">
         <v>104</v>
       </c>
@@ -28615,7 +28650,7 @@
       </c>
       <c r="H28" s="98"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:19">
       <c r="A29" s="122" t="s">
         <v>105</v>
       </c>
@@ -28640,7 +28675,7 @@
       </c>
       <c r="H29" s="98"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:19">
       <c r="A30" s="122" t="s">
         <v>107</v>
       </c>
@@ -28665,7 +28700,7 @@
       </c>
       <c r="H30" s="98"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:19">
       <c r="A31" s="122" t="s">
         <v>107</v>
       </c>
@@ -28690,7 +28725,7 @@
       </c>
       <c r="H31" s="98"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:19" hidden="1">
       <c r="A32" s="122" t="s">
         <v>108</v>
       </c>
@@ -28715,7 +28750,7 @@
       </c>
       <c r="H32" s="98"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" s="122" t="s">
         <v>108</v>
       </c>
@@ -28765,7 +28800,7 @@
       </c>
       <c r="H34" s="98"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="122" t="s">
         <v>113</v>
       </c>
@@ -28786,7 +28821,7 @@
       <c r="G35" s="122"/>
       <c r="H35" s="98"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="122" t="s">
         <v>115</v>
       </c>
@@ -28807,7 +28842,7 @@
       <c r="G36" s="122"/>
       <c r="H36" s="98"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="122" t="s">
         <v>116</v>
       </c>
@@ -28828,7 +28863,7 @@
       <c r="G37" s="122"/>
       <c r="H37" s="98"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="122" t="s">
         <v>118</v>
       </c>
@@ -28849,7 +28884,7 @@
       <c r="G38" s="122"/>
       <c r="H38" s="98"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="122" t="s">
         <v>119</v>
       </c>
@@ -28870,7 +28905,7 @@
       <c r="G39" s="122"/>
       <c r="H39" s="98"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40" s="122" t="s">
         <v>119</v>
       </c>
@@ -28891,7 +28926,7 @@
       <c r="G40" s="122"/>
       <c r="H40" s="98"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="122" t="s">
         <v>120</v>
       </c>
@@ -28912,7 +28947,7 @@
       <c r="G41" s="122"/>
       <c r="H41" s="98"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="122" t="s">
         <v>123</v>
       </c>
@@ -28933,7 +28968,7 @@
       <c r="G42" s="122"/>
       <c r="H42" s="98"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" hidden="1">
       <c r="A43" s="122" t="s">
         <v>124</v>
       </c>
@@ -28954,7 +28989,7 @@
       <c r="G43" s="122"/>
       <c r="H43" s="98"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" hidden="1">
       <c r="A44" s="122" t="s">
         <v>125</v>
       </c>
@@ -28975,7 +29010,7 @@
       <c r="G44" s="122"/>
       <c r="H44" s="98"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" hidden="1">
       <c r="A45" s="122" t="s">
         <v>126</v>
       </c>
@@ -28996,7 +29031,7 @@
       <c r="G45" s="122"/>
       <c r="H45" s="98"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="122" t="s">
         <v>127</v>
       </c>
@@ -29017,7 +29052,7 @@
       <c r="G46" s="122"/>
       <c r="H46" s="98"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47" s="122" t="s">
         <v>128</v>
       </c>
@@ -29038,7 +29073,7 @@
       <c r="G47" s="122"/>
       <c r="H47" s="98"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="122" t="s">
         <v>128</v>
       </c>
@@ -29061,7 +29096,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" hidden="1">
       <c r="A49" s="122" t="s">
         <v>131</v>
       </c>
@@ -29082,7 +29117,7 @@
       <c r="G49" s="122"/>
       <c r="H49" s="98"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" hidden="1">
       <c r="A50" s="122" t="s">
         <v>132</v>
       </c>
@@ -29103,7 +29138,7 @@
       <c r="G50" s="122"/>
       <c r="H50" s="98"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1">
       <c r="A51" s="122" t="s">
         <v>133</v>
       </c>
@@ -29124,7 +29159,7 @@
       <c r="G51" s="122"/>
       <c r="H51" s="98"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" hidden="1">
       <c r="A52" s="122" t="s">
         <v>134</v>
       </c>
@@ -29145,7 +29180,7 @@
       <c r="G52" s="122"/>
       <c r="H52" s="98"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1">
       <c r="A53" s="122" t="s">
         <v>137</v>
       </c>
@@ -29166,7 +29201,7 @@
       <c r="G53" s="122"/>
       <c r="H53" s="98"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1">
       <c r="C54" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29174,7 +29209,7 @@
       <c r="G54" s="98"/>
       <c r="H54" s="98"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1">
       <c r="C55" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29182,14 +29217,14 @@
       <c r="G55" s="98"/>
       <c r="H55" s="98"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" hidden="1">
       <c r="C56" s="72" t="s">
         <v>136</v>
       </c>
       <c r="G56" s="98"/>
       <c r="H56" s="98"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" hidden="1">
       <c r="C57" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29197,7 +29232,7 @@
       <c r="G57" s="98"/>
       <c r="H57" s="98"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" hidden="1">
       <c r="C58" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29205,7 +29240,7 @@
       <c r="G58" s="98"/>
       <c r="H58" s="98"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" hidden="1">
       <c r="C59" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29213,7 +29248,7 @@
       <c r="G59" s="98"/>
       <c r="H59" s="98"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" hidden="1">
       <c r="C60" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29221,7 +29256,7 @@
       <c r="G60" s="98"/>
       <c r="H60" s="98"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" hidden="1">
       <c r="C61" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29229,7 +29264,7 @@
       <c r="G61" s="98"/>
       <c r="H61" s="98"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" hidden="1">
       <c r="C62" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29270,9 +29305,19 @@
       <c r="B79" s="72"/>
     </row>
   </sheetData>
-  <sortState ref="E7:E32">
-    <sortCondition ref="E2:E64"/>
-  </sortState>
+  <autoFilter ref="A1:H62">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Sylvania QHE4X32T8/UNV ISL-SC"/>
+        <filter val="Sylvania QHE4X32T8/UNV ISN-SC"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -29283,41 +29328,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="98" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="98" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="98" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="98" customWidth="1"/>
-    <col min="5" max="256" width="9.140625" style="98" customWidth="1"/>
-    <col min="257" max="16384" width="8.85546875" style="26"/>
+    <col min="1" max="1" width="13.88671875" style="98" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="98" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="98" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" style="98" customWidth="1"/>
+    <col min="5" max="256" width="9.109375" style="98" customWidth="1"/>
+    <col min="257" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="87" customHeight="1">
       <c r="A1" s="124"/>
-      <c r="B1" s="184" t="s">
+      <c r="B1" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="186"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="169"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="170" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="171"/>
-      <c r="C2" s="182" t="s">
+      <c r="C2" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="183"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="178"/>
-      <c r="B3" s="180"/>
-      <c r="C3" s="181" t="s">
+      <c r="A3" s="174"/>
+      <c r="B3" s="175"/>
+      <c r="C3" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="183"/>
+      <c r="D3" s="173"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
@@ -29334,272 +29379,272 @@
         <f>IF('Audit Master'!L80=0, "", 'Audit Master'!L80)</f>
         <v/>
       </c>
-      <c r="B5" s="187" t="str">
+      <c r="B5" s="164" t="str">
         <f>IF(A5="", "", "Philips 40820-3")</f>
         <v/>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="189"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="166"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="125" t="str">
         <f>IF('Audit Master'!M80=0, "", 'Audit Master'!M80)</f>
         <v/>
       </c>
-      <c r="B6" s="187" t="str">
+      <c r="B6" s="164" t="str">
         <f>IF(A6="", "", "TCP 20714")</f>
         <v/>
       </c>
-      <c r="C6" s="188"/>
-      <c r="D6" s="189"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="166"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="125" t="str">
         <f>IF('Audit Master'!N80=0, "", 'Audit Master'!N80)</f>
         <v/>
       </c>
-      <c r="B7" s="187" t="str">
+      <c r="B7" s="164" t="str">
         <f>IF(A7="", "", "Sylvania F017XP")</f>
         <v/>
       </c>
-      <c r="C7" s="188"/>
-      <c r="D7" s="189"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="166"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="126" t="str">
         <f>IF('Audit Master'!O80=0, "", 'Audit Master'!O80)</f>
         <v/>
       </c>
-      <c r="B8" s="187" t="str">
+      <c r="B8" s="164" t="str">
         <f>IF(A8="", "", "Sylvania F028SS")</f>
         <v/>
       </c>
-      <c r="C8" s="188"/>
-      <c r="D8" s="189"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="166"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="126" t="str">
         <f>IF('Audit Master'!P80=0, "", 'Audit Master'!P80)</f>
         <v/>
       </c>
-      <c r="B9" s="187" t="str">
+      <c r="B9" s="164" t="str">
         <f>IF(A9="", "", "Sylvania F032XP")</f>
         <v/>
       </c>
-      <c r="C9" s="188"/>
-      <c r="D9" s="189"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="166"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="126" t="str">
         <f>IF('Audit Master'!Q80=0, "", 'Audit Master'!Q80)</f>
         <v/>
       </c>
-      <c r="B10" s="187" t="str">
+      <c r="B10" s="164" t="str">
         <f>IF(A10="", "", "Sylvania FB030")</f>
         <v/>
       </c>
-      <c r="C10" s="188"/>
-      <c r="D10" s="189"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="166"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="126" t="str">
         <f>IF('Audit Master'!R80=0, "", 'Audit Master'!R80)</f>
         <v/>
       </c>
-      <c r="B11" s="187" t="str">
+      <c r="B11" s="164" t="str">
         <f>IF(A11="", "", "TCP 33123SP")</f>
         <v/>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="189"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="166"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="126" t="str">
         <f>IF('Audit Master'!S80=0, "", 'Audit Master'!S80)</f>
         <v/>
       </c>
-      <c r="B12" s="187" t="str">
+      <c r="B12" s="164" t="str">
         <f>IF(A12="", "", "TCP 33113SP")</f>
         <v/>
       </c>
-      <c r="C12" s="188"/>
-      <c r="D12" s="189"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="166"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="126" t="str">
         <f>IF('Audit Master'!T80=0, "", 'Audit Master'!T80)</f>
         <v/>
       </c>
-      <c r="B13" s="187" t="str">
+      <c r="B13" s="164" t="str">
         <f>IF(A13="", "", "Philips 40877-3")</f>
         <v/>
       </c>
-      <c r="C13" s="188"/>
-      <c r="D13" s="189"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="166"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="126" t="str">
         <f>IF('Audit Master'!U80=0, "", 'Audit Master'!U80)</f>
         <v/>
       </c>
-      <c r="B14" s="187" t="str">
+      <c r="B14" s="164" t="str">
         <f>IF(A14="", "", "TCP 33213SSP")</f>
         <v/>
       </c>
-      <c r="C14" s="188"/>
-      <c r="D14" s="189"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="166"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="126" t="str">
         <f>IF('Audit Master'!V80=0, "", 'Audit Master'!V80)</f>
         <v/>
       </c>
-      <c r="B15" s="187" t="str">
+      <c r="B15" s="164" t="str">
         <f>IF(A15="", "", "Sylvania FP54T5HO")</f>
         <v/>
       </c>
-      <c r="C15" s="188"/>
-      <c r="D15" s="189"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="166"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="127" t="str">
         <f>IF('Audit Master'!W80=0, "", 'Audit Master'!W80)</f>
         <v/>
       </c>
-      <c r="B16" s="187" t="str">
+      <c r="B16" s="164" t="str">
         <f>IF(A16="", "", "Sylvania QHE2X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C16" s="188"/>
-      <c r="D16" s="189"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="166"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="126" t="str">
         <f>IF('Audit Master'!X80=0, "", 'Audit Master'!X80)</f>
         <v/>
       </c>
-      <c r="B17" s="187" t="str">
+      <c r="B17" s="164" t="str">
         <f>IF(A17="", "", "Sylvania QHE4X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C17" s="188"/>
-      <c r="D17" s="189"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="166"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="126" t="str">
         <f>IF('Audit Master'!Y80=0, "", 'Audit Master'!Y80)</f>
         <v/>
       </c>
-      <c r="B18" s="187" t="str">
+      <c r="B18" s="164" t="str">
         <f>IF(A18="", "", "Sylvania QHE4X32T8/UNV ISN-SC")</f>
         <v/>
       </c>
-      <c r="C18" s="188"/>
-      <c r="D18" s="189"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="166"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="128" t="str">
         <f>IF('Audit Master'!Z80=0, "", 'Audit Master'!Z80)</f>
         <v/>
       </c>
-      <c r="B19" s="187" t="str">
+      <c r="B19" s="164" t="str">
         <f>IF(A19="", "", "Sylvania QHE4X32T8/UNV ISH")</f>
         <v/>
       </c>
-      <c r="C19" s="188"/>
-      <c r="D19" s="189"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="166"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="181"/>
-      <c r="B20" s="182"/>
-      <c r="C20" s="182"/>
-      <c r="D20" s="183"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="173"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="175" t="s">
+      <c r="A21" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="176"/>
-      <c r="C21" s="176"/>
-      <c r="D21" s="177"/>
+      <c r="B21" s="181"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="182"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="164"/>
-      <c r="B22" s="165"/>
-      <c r="C22" s="165"/>
-      <c r="D22" s="166"/>
+      <c r="A22" s="183"/>
+      <c r="B22" s="184"/>
+      <c r="C22" s="184"/>
+      <c r="D22" s="185"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="164"/>
-      <c r="B23" s="165"/>
-      <c r="C23" s="165"/>
-      <c r="D23" s="166"/>
+      <c r="A23" s="183"/>
+      <c r="B23" s="184"/>
+      <c r="C23" s="184"/>
+      <c r="D23" s="185"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="172"/>
-      <c r="B24" s="173"/>
-      <c r="C24" s="173"/>
-      <c r="D24" s="174"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="178"/>
+      <c r="C24" s="178"/>
+      <c r="D24" s="179"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="169" t="s">
+      <c r="A25" s="170" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="170"/>
-      <c r="C25" s="170"/>
+      <c r="B25" s="188"/>
+      <c r="C25" s="188"/>
       <c r="D25" s="171"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="172"/>
-      <c r="B26" s="173"/>
-      <c r="C26" s="173"/>
-      <c r="D26" s="174"/>
+      <c r="A26" s="177"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="179"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="169" t="s">
+      <c r="A27" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
       <c r="D27" s="171"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="175"/>
-      <c r="B28" s="176"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="177"/>
+      <c r="A28" s="180"/>
+      <c r="B28" s="181"/>
+      <c r="C28" s="181"/>
+      <c r="D28" s="182"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="178"/>
-      <c r="B29" s="179"/>
-      <c r="C29" s="179"/>
-      <c r="D29" s="180"/>
+      <c r="A29" s="174"/>
+      <c r="B29" s="189"/>
+      <c r="C29" s="189"/>
+      <c r="D29" s="175"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="169" t="s">
+      <c r="A30" s="170" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="170"/>
-      <c r="C30" s="170"/>
+      <c r="B30" s="188"/>
+      <c r="C30" s="188"/>
       <c r="D30" s="171"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="164"/>
-      <c r="B31" s="165"/>
-      <c r="C31" s="165"/>
-      <c r="D31" s="166"/>
+      <c r="A31" s="183"/>
+      <c r="B31" s="184"/>
+      <c r="C31" s="184"/>
+      <c r="D31" s="185"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="164"/>
-      <c r="B32" s="165"/>
-      <c r="C32" s="165"/>
-      <c r="D32" s="166"/>
+      <c r="A32" s="183"/>
+      <c r="B32" s="184"/>
+      <c r="C32" s="184"/>
+      <c r="D32" s="185"/>
     </row>
     <row r="33" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A33" s="167" t="s">
+      <c r="A33" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="168"/>
+      <c r="B33" s="187"/>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
         <v>55</v>
@@ -29627,18 +29672,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
@@ -29652,15 +29694,18 @@
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Hide rows in work order
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -4358,6 +4358,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="49" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4505,10 +4509,6 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2059">
     <cellStyle name="20% - Accent1 2" xfId="33"/>
@@ -22300,14 +22300,14 @@
       <c r="R4" s="130"/>
     </row>
     <row r="5" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A5" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="148"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
+      <c r="A5" s="151" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="152"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
       <c r="G5" s="44" t="s">
         <v>139</v>
       </c>
@@ -22319,14 +22319,14 @@
       <c r="R5" s="135"/>
     </row>
     <row r="6" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A6" s="147" t="s">
+      <c r="A6" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="148"/>
-      <c r="C6" s="161"/>
-      <c r="D6" s="161"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
       <c r="G6" s="44"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
@@ -22336,16 +22336,16 @@
       <c r="R6" s="135"/>
     </row>
     <row r="7" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="151" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="161" t="s">
+      <c r="B7" s="152"/>
+      <c r="C7" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="G7" s="44" t="s">
         <v>39</v>
       </c>
@@ -22358,16 +22358,16 @@
       <c r="AA7" s="130"/>
     </row>
     <row r="8" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="162" t="s">
+      <c r="B8" s="152"/>
+      <c r="C8" s="166" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="162"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="162"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
       <c r="G8" s="51" t="s">
         <v>43</v>
       </c>
@@ -22426,18 +22426,18 @@
         <v>4</v>
       </c>
       <c r="E12" s="61"/>
-      <c r="F12" s="143" t="s">
+      <c r="F12" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="148"/>
       <c r="I12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="143" t="s">
+      <c r="J12" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="163"/>
+      <c r="K12" s="167"/>
       <c r="L12" s="63"/>
       <c r="AA12" s="130"/>
     </row>
@@ -23439,7 +23439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="29.4" customHeight="1">
+    <row r="26" spans="1:27" ht="29.4" customHeight="1" thickBot="1">
       <c r="A26" s="74">
         <v>13</v>
       </c>
@@ -23514,7 +23514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="29.4" customHeight="1">
+    <row r="27" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A27" s="74">
         <v>14</v>
       </c>
@@ -23589,7 +23589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="29.4" customHeight="1">
+    <row r="28" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A28" s="74">
         <v>15</v>
       </c>
@@ -23664,7 +23664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="29.4" customHeight="1">
+    <row r="29" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A29" s="74">
         <v>16</v>
       </c>
@@ -23739,7 +23739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="29.4" customHeight="1">
+    <row r="30" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A30" s="74">
         <v>17</v>
       </c>
@@ -23814,7 +23814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="29.4" customHeight="1">
+    <row r="31" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A31" s="74">
         <v>18</v>
       </c>
@@ -23889,7 +23889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="29.4" customHeight="1">
+    <row r="32" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A32" s="74">
         <v>19</v>
       </c>
@@ -23964,7 +23964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="29.4" customHeight="1">
+    <row r="33" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A33" s="74">
         <v>20</v>
       </c>
@@ -24039,7 +24039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="29.4" customHeight="1">
+    <row r="34" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A34" s="74">
         <v>21</v>
       </c>
@@ -24114,7 +24114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="29.4" customHeight="1">
+    <row r="35" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A35" s="74">
         <v>22</v>
       </c>
@@ -24189,7 +24189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="29.4" customHeight="1">
+    <row r="36" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A36" s="74">
         <v>23</v>
       </c>
@@ -24264,7 +24264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="29.4" customHeight="1">
+    <row r="37" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A37" s="74">
         <v>24</v>
       </c>
@@ -24339,7 +24339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="29.4" customHeight="1">
+    <row r="38" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A38" s="74">
         <v>25</v>
       </c>
@@ -24414,7 +24414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="29.4" customHeight="1">
+    <row r="39" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A39" s="74">
         <v>26</v>
       </c>
@@ -24489,7 +24489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="29.4" customHeight="1">
+    <row r="40" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A40" s="74">
         <v>27</v>
       </c>
@@ -24564,7 +24564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="29.4" customHeight="1">
+    <row r="41" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A41" s="74">
         <v>28</v>
       </c>
@@ -24639,7 +24639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="29.4" customHeight="1">
+    <row r="42" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A42" s="74">
         <v>29</v>
       </c>
@@ -24714,7 +24714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="29.4" customHeight="1">
+    <row r="43" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A43" s="74">
         <v>30</v>
       </c>
@@ -24789,7 +24789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="29.4" customHeight="1">
+    <row r="44" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A44" s="74">
         <v>31</v>
       </c>
@@ -24864,7 +24864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="29.4" customHeight="1">
+    <row r="45" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A45" s="74">
         <v>32</v>
       </c>
@@ -24939,7 +24939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="29.4" customHeight="1">
+    <row r="46" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A46" s="74">
         <v>33</v>
       </c>
@@ -25014,7 +25014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="29.4" customHeight="1">
+    <row r="47" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A47" s="74">
         <v>34</v>
       </c>
@@ -25089,7 +25089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="29.4" customHeight="1">
+    <row r="48" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A48" s="74">
         <v>35</v>
       </c>
@@ -25164,7 +25164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="29.4" customHeight="1">
+    <row r="49" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A49" s="74">
         <v>36</v>
       </c>
@@ -25239,7 +25239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="29.4" customHeight="1">
+    <row r="50" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A50" s="74">
         <v>37</v>
       </c>
@@ -25314,7 +25314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="29.4" customHeight="1">
+    <row r="51" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A51" s="74">
         <v>38</v>
       </c>
@@ -25390,7 +25390,7 @@
       </c>
       <c r="AA51" s="130"/>
     </row>
-    <row r="52" spans="1:27" ht="29.4" customHeight="1">
+    <row r="52" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A52" s="74">
         <v>39</v>
       </c>
@@ -25465,7 +25465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="29.4" customHeight="1">
+    <row r="53" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A53" s="74">
         <v>40</v>
       </c>
@@ -25540,7 +25540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="29.4" customHeight="1">
+    <row r="54" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A54" s="74">
         <v>41</v>
       </c>
@@ -25615,7 +25615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="29.4" customHeight="1">
+    <row r="55" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A55" s="74">
         <v>42</v>
       </c>
@@ -25690,7 +25690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="29.4" customHeight="1">
+    <row r="56" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A56" s="74">
         <v>43</v>
       </c>
@@ -25765,7 +25765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="29.4" customHeight="1">
+    <row r="57" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A57" s="74">
         <v>44</v>
       </c>
@@ -25840,7 +25840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="29.4" customHeight="1">
+    <row r="58" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A58" s="74">
         <v>45</v>
       </c>
@@ -25915,7 +25915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="29.4" customHeight="1">
+    <row r="59" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A59" s="74">
         <v>46</v>
       </c>
@@ -25990,7 +25990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="29.4" customHeight="1">
+    <row r="60" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A60" s="74">
         <v>47</v>
       </c>
@@ -26065,7 +26065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="29.4" customHeight="1">
+    <row r="61" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A61" s="74">
         <v>48</v>
       </c>
@@ -26140,7 +26140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="29.4" customHeight="1">
+    <row r="62" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A62" s="74">
         <v>49</v>
       </c>
@@ -26215,7 +26215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="29.4" customHeight="1">
+    <row r="63" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A63" s="74">
         <v>50</v>
       </c>
@@ -26290,7 +26290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="29.4" customHeight="1">
+    <row r="64" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A64" s="74">
         <v>51</v>
       </c>
@@ -26365,7 +26365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="29.4" customHeight="1">
+    <row r="65" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A65" s="74">
         <v>52</v>
       </c>
@@ -26440,7 +26440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="29.4" customHeight="1">
+    <row r="66" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A66" s="74">
         <v>53</v>
       </c>
@@ -26515,7 +26515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="29.4" customHeight="1">
+    <row r="67" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A67" s="74">
         <v>54</v>
       </c>
@@ -26590,7 +26590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="29.4" customHeight="1">
+    <row r="68" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A68" s="74">
         <v>55</v>
       </c>
@@ -26665,7 +26665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="29.4" customHeight="1">
+    <row r="69" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A69" s="74">
         <v>56</v>
       </c>
@@ -26740,7 +26740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="29.4" customHeight="1">
+    <row r="70" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A70" s="74">
         <v>57</v>
       </c>
@@ -26815,7 +26815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="29.4" customHeight="1">
+    <row r="71" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A71" s="74">
         <v>58</v>
       </c>
@@ -26890,7 +26890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="29.4" customHeight="1">
+    <row r="72" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A72" s="74">
         <v>59</v>
       </c>
@@ -26965,7 +26965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="29.4" customHeight="1">
+    <row r="73" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A73" s="74">
         <v>60</v>
       </c>
@@ -27040,7 +27040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="29.4" customHeight="1">
+    <row r="74" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A74" s="74">
         <v>61</v>
       </c>
@@ -27115,7 +27115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="29.4" customHeight="1">
+    <row r="75" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A75" s="74">
         <v>62</v>
       </c>
@@ -27190,7 +27190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="29.4" customHeight="1">
+    <row r="76" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A76" s="74">
         <v>63</v>
       </c>
@@ -27265,7 +27265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="29.4" customHeight="1">
+    <row r="77" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A77" s="74">
         <v>64</v>
       </c>
@@ -27340,7 +27340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="29.4" customHeight="1">
+    <row r="78" spans="1:26" ht="29.4" hidden="1" customHeight="1">
       <c r="A78" s="74">
         <v>65</v>
       </c>
@@ -27415,7 +27415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="29.4" customHeight="1" thickBot="1">
+    <row r="79" spans="1:26" ht="29.4" hidden="1" customHeight="1" thickBot="1">
       <c r="A79" s="74">
         <v>66</v>
       </c>
@@ -27614,29 +27614,29 @@
       <c r="K83" s="6"/>
     </row>
     <row r="84" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A84" s="151"/>
-      <c r="B84" s="152"/>
+      <c r="A84" s="155"/>
+      <c r="B84" s="156"/>
       <c r="C84" s="97"/>
       <c r="D84" s="97"/>
       <c r="E84" s="97"/>
-      <c r="F84" s="152"/>
-      <c r="G84" s="152"/>
+      <c r="F84" s="156"/>
+      <c r="G84" s="156"/>
       <c r="H84" s="97"/>
       <c r="I84" s="97"/>
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A85" s="141" t="s">
+      <c r="A85" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="142"/>
+      <c r="B85" s="146"/>
       <c r="C85" s="100"/>
       <c r="D85" s="100"/>
       <c r="E85" s="100"/>
-      <c r="F85" s="142" t="s">
+      <c r="F85" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="142"/>
+      <c r="G85" s="146"/>
       <c r="J85" s="7" t="s">
         <v>35</v>
       </c>
@@ -27651,10 +27651,10 @@
       <c r="E86" s="102"/>
       <c r="F86" s="102"/>
       <c r="G86" s="102"/>
-      <c r="J86" s="153" t="s">
+      <c r="J86" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="K86" s="154"/>
+      <c r="K86" s="158"/>
       <c r="L86" s="30"/>
     </row>
     <row r="87" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
@@ -27665,40 +27665,40 @@
       <c r="E87" s="102"/>
       <c r="F87" s="102"/>
       <c r="G87" s="102"/>
-      <c r="J87" s="155"/>
-      <c r="K87" s="156"/>
+      <c r="J87" s="159"/>
+      <c r="K87" s="160"/>
       <c r="L87" s="30"/>
     </row>
     <row r="88" spans="1:12" s="98" customFormat="1" ht="22.95" customHeight="1" thickBot="1">
-      <c r="A88" s="149"/>
-      <c r="B88" s="150"/>
+      <c r="A88" s="153"/>
+      <c r="B88" s="154"/>
       <c r="C88" s="103"/>
       <c r="D88" s="103"/>
       <c r="E88" s="103"/>
-      <c r="F88" s="150"/>
-      <c r="G88" s="150"/>
+      <c r="F88" s="154"/>
+      <c r="G88" s="154"/>
       <c r="H88" s="97"/>
       <c r="I88" s="97"/>
-      <c r="J88" s="157" t="s">
+      <c r="J88" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="K88" s="158"/>
+      <c r="K88" s="162"/>
       <c r="L88" s="104"/>
     </row>
     <row r="89" spans="1:12" s="98" customFormat="1" ht="17.399999999999999" customHeight="1">
-      <c r="A89" s="141" t="s">
+      <c r="A89" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="142"/>
+      <c r="B89" s="146"/>
       <c r="C89" s="100"/>
       <c r="D89" s="100"/>
       <c r="E89" s="100"/>
-      <c r="F89" s="142" t="s">
+      <c r="F89" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="G89" s="142"/>
-      <c r="J89" s="159"/>
-      <c r="K89" s="160"/>
+      <c r="G89" s="146"/>
+      <c r="J89" s="163"/>
+      <c r="K89" s="164"/>
       <c r="L89" s="104"/>
     </row>
     <row r="90" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1">
@@ -27732,17 +27732,17 @@
       <c r="L91" s="110"/>
     </row>
     <row r="92" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A92" s="145" t="s">
+      <c r="A92" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="B92" s="146"/>
+      <c r="B92" s="150"/>
       <c r="C92" s="111"/>
       <c r="D92" s="111"/>
       <c r="E92" s="111"/>
-      <c r="F92" s="146" t="s">
+      <c r="F92" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="G92" s="146"/>
+      <c r="G92" s="150"/>
       <c r="H92" s="112"/>
       <c r="I92" s="113"/>
       <c r="J92" s="114" t="s">
@@ -27794,7 +27794,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="21" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup scale="56" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -28533,10 +28533,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="98"/>
-      <c r="Q24" s="192" t="s">
+      <c r="Q24" s="143" t="s">
         <v>104</v>
       </c>
-      <c r="R24" s="193" t="s">
+      <c r="R24" s="144" t="s">
         <v>142</v>
       </c>
       <c r="S24" s="26" t="str">
@@ -28573,7 +28573,7 @@
       <c r="A26" s="123" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="190" t="s">
+      <c r="B26" s="141" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="72" t="str">
@@ -28586,7 +28586,7 @@
       <c r="E26" s="123">
         <v>4</v>
       </c>
-      <c r="F26" s="191" t="s">
+      <c r="F26" s="142" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="122">
@@ -29326,7 +29326,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -29340,29 +29342,29 @@
   <sheetData>
     <row r="1" spans="1:4" ht="87" customHeight="1">
       <c r="A1" s="124"/>
-      <c r="B1" s="167" t="s">
+      <c r="B1" s="171" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="168"/>
-      <c r="D1" s="169"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="173"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="174" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="172" t="s">
+      <c r="B2" s="175"/>
+      <c r="C2" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="173"/>
+      <c r="D2" s="177"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="174"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="176" t="s">
+      <c r="A3" s="178"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="180" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="173"/>
+      <c r="D3" s="177"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
@@ -29379,272 +29381,272 @@
         <f>IF('Audit Master'!L80=0, "", 'Audit Master'!L80)</f>
         <v/>
       </c>
-      <c r="B5" s="164" t="str">
+      <c r="B5" s="168" t="str">
         <f>IF(A5="", "", "Philips 40820-3")</f>
         <v/>
       </c>
-      <c r="C5" s="165"/>
-      <c r="D5" s="166"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="170"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="125" t="str">
         <f>IF('Audit Master'!M80=0, "", 'Audit Master'!M80)</f>
         <v/>
       </c>
-      <c r="B6" s="164" t="str">
+      <c r="B6" s="168" t="str">
         <f>IF(A6="", "", "TCP 20714")</f>
         <v/>
       </c>
-      <c r="C6" s="165"/>
-      <c r="D6" s="166"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="170"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="125" t="str">
         <f>IF('Audit Master'!N80=0, "", 'Audit Master'!N80)</f>
         <v/>
       </c>
-      <c r="B7" s="164" t="str">
+      <c r="B7" s="168" t="str">
         <f>IF(A7="", "", "Sylvania F017XP")</f>
         <v/>
       </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="166"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="170"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="126" t="str">
         <f>IF('Audit Master'!O80=0, "", 'Audit Master'!O80)</f>
         <v/>
       </c>
-      <c r="B8" s="164" t="str">
+      <c r="B8" s="168" t="str">
         <f>IF(A8="", "", "Sylvania F028SS")</f>
         <v/>
       </c>
-      <c r="C8" s="165"/>
-      <c r="D8" s="166"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="170"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="126" t="str">
         <f>IF('Audit Master'!P80=0, "", 'Audit Master'!P80)</f>
         <v/>
       </c>
-      <c r="B9" s="164" t="str">
+      <c r="B9" s="168" t="str">
         <f>IF(A9="", "", "Sylvania F032XP")</f>
         <v/>
       </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="166"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="170"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="126" t="str">
         <f>IF('Audit Master'!Q80=0, "", 'Audit Master'!Q80)</f>
         <v/>
       </c>
-      <c r="B10" s="164" t="str">
+      <c r="B10" s="168" t="str">
         <f>IF(A10="", "", "Sylvania FB030")</f>
         <v/>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="166"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="170"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="126" t="str">
         <f>IF('Audit Master'!R80=0, "", 'Audit Master'!R80)</f>
         <v/>
       </c>
-      <c r="B11" s="164" t="str">
+      <c r="B11" s="168" t="str">
         <f>IF(A11="", "", "TCP 33123SP")</f>
         <v/>
       </c>
-      <c r="C11" s="165"/>
-      <c r="D11" s="166"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="170"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="126" t="str">
         <f>IF('Audit Master'!S80=0, "", 'Audit Master'!S80)</f>
         <v/>
       </c>
-      <c r="B12" s="164" t="str">
+      <c r="B12" s="168" t="str">
         <f>IF(A12="", "", "TCP 33113SP")</f>
         <v/>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="166"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="170"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="126" t="str">
         <f>IF('Audit Master'!T80=0, "", 'Audit Master'!T80)</f>
         <v/>
       </c>
-      <c r="B13" s="164" t="str">
+      <c r="B13" s="168" t="str">
         <f>IF(A13="", "", "Philips 40877-3")</f>
         <v/>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="166"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="126" t="str">
         <f>IF('Audit Master'!U80=0, "", 'Audit Master'!U80)</f>
         <v/>
       </c>
-      <c r="B14" s="164" t="str">
+      <c r="B14" s="168" t="str">
         <f>IF(A14="", "", "TCP 33213SSP")</f>
         <v/>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="166"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="170"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="126" t="str">
         <f>IF('Audit Master'!V80=0, "", 'Audit Master'!V80)</f>
         <v/>
       </c>
-      <c r="B15" s="164" t="str">
+      <c r="B15" s="168" t="str">
         <f>IF(A15="", "", "Sylvania FP54T5HO")</f>
         <v/>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="166"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="170"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="127" t="str">
         <f>IF('Audit Master'!W80=0, "", 'Audit Master'!W80)</f>
         <v/>
       </c>
-      <c r="B16" s="164" t="str">
+      <c r="B16" s="168" t="str">
         <f>IF(A16="", "", "Sylvania QHE2X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="166"/>
+      <c r="C16" s="169"/>
+      <c r="D16" s="170"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="126" t="str">
         <f>IF('Audit Master'!X80=0, "", 'Audit Master'!X80)</f>
         <v/>
       </c>
-      <c r="B17" s="164" t="str">
+      <c r="B17" s="168" t="str">
         <f>IF(A17="", "", "Sylvania QHE4X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="166"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="170"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="126" t="str">
         <f>IF('Audit Master'!Y80=0, "", 'Audit Master'!Y80)</f>
         <v/>
       </c>
-      <c r="B18" s="164" t="str">
+      <c r="B18" s="168" t="str">
         <f>IF(A18="", "", "Sylvania QHE4X32T8/UNV ISN-SC")</f>
         <v/>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166"/>
+      <c r="C18" s="169"/>
+      <c r="D18" s="170"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="128" t="str">
         <f>IF('Audit Master'!Z80=0, "", 'Audit Master'!Z80)</f>
         <v/>
       </c>
-      <c r="B19" s="164" t="str">
+      <c r="B19" s="168" t="str">
         <f>IF(A19="", "", "Sylvania QHE4X32T8/UNV ISH")</f>
         <v/>
       </c>
-      <c r="C19" s="165"/>
-      <c r="D19" s="166"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="170"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="176"/>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
+      <c r="A20" s="180"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="176"/>
+      <c r="D20" s="177"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="180" t="s">
+      <c r="A21" s="184" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="182"/>
+      <c r="B21" s="185"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="183"/>
-      <c r="B22" s="184"/>
-      <c r="C22" s="184"/>
-      <c r="D22" s="185"/>
+      <c r="A22" s="187"/>
+      <c r="B22" s="188"/>
+      <c r="C22" s="188"/>
+      <c r="D22" s="189"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="183"/>
-      <c r="B23" s="184"/>
-      <c r="C23" s="184"/>
-      <c r="D23" s="185"/>
+      <c r="A23" s="187"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="189"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="177"/>
-      <c r="B24" s="178"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="179"/>
+      <c r="A24" s="181"/>
+      <c r="B24" s="182"/>
+      <c r="C24" s="182"/>
+      <c r="D24" s="183"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="170" t="s">
+      <c r="A25" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="188"/>
-      <c r="C25" s="188"/>
-      <c r="D25" s="171"/>
+      <c r="B25" s="192"/>
+      <c r="C25" s="192"/>
+      <c r="D25" s="175"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="177"/>
-      <c r="B26" s="178"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="179"/>
+      <c r="A26" s="181"/>
+      <c r="B26" s="182"/>
+      <c r="C26" s="182"/>
+      <c r="D26" s="183"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="170" t="s">
+      <c r="A27" s="174" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="188"/>
-      <c r="C27" s="188"/>
-      <c r="D27" s="171"/>
+      <c r="B27" s="192"/>
+      <c r="C27" s="192"/>
+      <c r="D27" s="175"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="180"/>
-      <c r="B28" s="181"/>
-      <c r="C28" s="181"/>
-      <c r="D28" s="182"/>
+      <c r="A28" s="184"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="186"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="174"/>
-      <c r="B29" s="189"/>
-      <c r="C29" s="189"/>
-      <c r="D29" s="175"/>
+      <c r="A29" s="178"/>
+      <c r="B29" s="193"/>
+      <c r="C29" s="193"/>
+      <c r="D29" s="179"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="170" t="s">
+      <c r="A30" s="174" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="188"/>
-      <c r="C30" s="188"/>
-      <c r="D30" s="171"/>
+      <c r="B30" s="192"/>
+      <c r="C30" s="192"/>
+      <c r="D30" s="175"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="183"/>
-      <c r="B31" s="184"/>
-      <c r="C31" s="184"/>
-      <c r="D31" s="185"/>
+      <c r="A31" s="187"/>
+      <c r="B31" s="188"/>
+      <c r="C31" s="188"/>
+      <c r="D31" s="189"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="183"/>
-      <c r="B32" s="184"/>
-      <c r="C32" s="184"/>
-      <c r="D32" s="185"/>
+      <c r="A32" s="187"/>
+      <c r="B32" s="188"/>
+      <c r="C32" s="188"/>
+      <c r="D32" s="189"/>
     </row>
     <row r="33" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A33" s="186" t="s">
+      <c r="A33" s="190" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="187"/>
+      <c r="B33" s="191"/>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Fixing up Work Order
added sensors
</commit_message>
<xml_diff>
--- a/Work Order - Lighting.xlsx
+++ b/Work Order - Lighting.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Audit Master" sheetId="1" r:id="rId1"/>
-    <sheet name="LightToParts" sheetId="4" r:id="rId2"/>
+    <sheet name="LightToParts" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="Andrey" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
@@ -84,6 +84,7 @@
     <definedName name="Other">#REF!</definedName>
     <definedName name="Payback_Per_Fixture_In_Months">#REF!</definedName>
     <definedName name="Percent_Occupancy">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Andrey!$A$1:$D$36</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Audit Master'!$A$1:$K$93</definedName>
     <definedName name="Project_Management">#REF!</definedName>
     <definedName name="PropCodes">'[1]Proposed Code'!$B$2:$F$1752</definedName>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
   <si>
     <t>Business Name:</t>
   </si>
@@ -553,10 +554,7 @@
     <t>Fluorescent, (3) 48", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
   </si>
   <si>
-    <t>Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
-  </si>
-  <si>
-    <t>Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</t>
+    <t>Occ Sensor</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1007,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1188,6 +1186,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1941,7 +1945,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2059">
+  <cellStyleXfs count="2060">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4041,8 +4045,9 @@
     <xf numFmtId="37" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="44" fillId="0" borderId="18" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="65" fillId="35" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4335,7 +4340,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4362,42 +4366,6 @@
     <xf numFmtId="0" fontId="69" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4428,46 +4396,67 @@
     <xf numFmtId="0" fontId="60" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4488,29 +4477,44 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2059">
+  <cellStyles count="2060">
     <cellStyle name="20% - Accent1 2" xfId="33"/>
     <cellStyle name="20% - Accent2 2" xfId="34"/>
     <cellStyle name="20% - Accent3 2" xfId="35"/>
@@ -6559,6 +6563,7 @@
     <cellStyle name="Percent 9" xfId="2049"/>
     <cellStyle name="SCL - Style1" xfId="27"/>
     <cellStyle name="SCLEntry" xfId="28"/>
+    <cellStyle name="Style 1" xfId="2059"/>
     <cellStyle name="Style 26" xfId="2050"/>
     <cellStyle name="Style 26 2" xfId="2051"/>
     <cellStyle name="Title 2" xfId="2052"/>
@@ -22228,7 +22233,7 @@
   </sheetPr>
   <dimension ref="A1:IM93"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -22246,7 +22251,8 @@
     <col min="12" max="12" width="15.88671875" style="1" customWidth="1"/>
     <col min="13" max="25" width="9.109375" style="1" customWidth="1"/>
     <col min="26" max="26" width="13.88671875" style="1" customWidth="1"/>
-    <col min="27" max="247" width="9.109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" style="1" customWidth="1"/>
+    <col min="28" max="247" width="9.109375" style="1" customWidth="1"/>
     <col min="248" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
@@ -22285,7 +22291,7 @@
       <c r="C3" s="38"/>
       <c r="F3" s="40"/>
       <c r="K3" s="6"/>
-      <c r="R3" s="130"/>
+      <c r="R3" s="129"/>
     </row>
     <row r="4" spans="1:27" ht="24" customHeight="1">
       <c r="A4" s="14" t="s">
@@ -22297,17 +22303,17 @@
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
       <c r="K4" s="6"/>
-      <c r="R4" s="130"/>
+      <c r="R4" s="129"/>
     </row>
     <row r="5" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A5" s="151" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="152"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
+      <c r="A5" s="161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="162"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
       <c r="G5" s="44" t="s">
         <v>139</v>
       </c>
@@ -22316,36 +22322,36 @@
       <c r="J5" s="45"/>
       <c r="K5" s="46"/>
       <c r="L5" s="47"/>
-      <c r="R5" s="135"/>
+      <c r="R5" s="134"/>
     </row>
     <row r="6" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A6" s="151" t="s">
+      <c r="A6" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="152"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="165"/>
-      <c r="F6" s="165"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="152"/>
+      <c r="E6" s="152"/>
+      <c r="F6" s="152"/>
       <c r="G6" s="44"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
       <c r="J6" s="45"/>
       <c r="K6" s="46"/>
       <c r="L6" s="47"/>
-      <c r="R6" s="135"/>
+      <c r="R6" s="134"/>
     </row>
     <row r="7" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="152"/>
-      <c r="C7" s="165" t="s">
+      <c r="B7" s="162"/>
+      <c r="C7" s="152" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
       <c r="G7" s="44" t="s">
         <v>39</v>
       </c>
@@ -22354,20 +22360,20 @@
       <c r="J7" s="48"/>
       <c r="K7" s="49"/>
       <c r="L7" s="50"/>
-      <c r="R7" s="135"/>
-      <c r="AA7" s="130"/>
+      <c r="R7" s="134"/>
+      <c r="AA7" s="129"/>
     </row>
     <row r="8" spans="1:27" ht="24.45" customHeight="1">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="152"/>
-      <c r="C8" s="166" t="s">
+      <c r="B8" s="162"/>
+      <c r="C8" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="153"/>
       <c r="G8" s="51" t="s">
         <v>43</v>
       </c>
@@ -22376,24 +22382,24 @@
       <c r="J8" s="48"/>
       <c r="K8" s="49"/>
       <c r="L8" s="50"/>
-      <c r="R8" s="130"/>
-      <c r="AA8" s="130"/>
+      <c r="R8" s="129"/>
+      <c r="AA8" s="129"/>
     </row>
     <row r="9" spans="1:27" ht="24.45" hidden="1" customHeight="1">
-      <c r="A9" s="136"/>
-      <c r="B9" s="137"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="139"/>
+      <c r="A9" s="135"/>
+      <c r="B9" s="136"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="138"/>
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="140"/>
+      <c r="K9" s="139"/>
       <c r="L9" s="50"/>
-      <c r="R9" s="130"/>
-      <c r="AA9" s="130"/>
+      <c r="R9" s="129"/>
+      <c r="AA9" s="129"/>
     </row>
     <row r="10" spans="1:27" ht="24.45" customHeight="1">
       <c r="A10" s="52"/>
@@ -22405,8 +22411,8 @@
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
       <c r="K10" s="6"/>
-      <c r="R10" s="130"/>
-      <c r="AA10" s="130"/>
+      <c r="R10" s="129"/>
+      <c r="AA10" s="129"/>
     </row>
     <row r="11" spans="1:27" ht="10.199999999999999" customHeight="1" thickBot="1">
       <c r="A11" s="56"/>
@@ -22415,8 +22421,8 @@
       <c r="E11" s="57"/>
       <c r="G11" s="2"/>
       <c r="K11" s="6"/>
-      <c r="R11" s="130"/>
-      <c r="AA11" s="130"/>
+      <c r="R11" s="129"/>
+      <c r="AA11" s="129"/>
     </row>
     <row r="12" spans="1:27" s="3" customFormat="1" ht="12" customHeight="1" thickTop="1">
       <c r="A12" s="58"/>
@@ -22426,20 +22432,20 @@
         <v>4</v>
       </c>
       <c r="E12" s="61"/>
-      <c r="F12" s="147" t="s">
+      <c r="F12" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="158"/>
       <c r="I12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="147" t="s">
+      <c r="J12" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="167"/>
+      <c r="K12" s="155"/>
       <c r="L12" s="63"/>
-      <c r="AA12" s="130"/>
+      <c r="AA12" s="129"/>
     </row>
     <row r="13" spans="1:27" s="3" customFormat="1" ht="57" customHeight="1">
       <c r="A13" s="64" t="s">
@@ -22473,52 +22479,54 @@
       <c r="K13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="133" t="s">
+      <c r="L13" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="133" t="s">
+      <c r="M13" s="132" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="133" t="s">
+      <c r="N13" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="O13" s="133" t="s">
+      <c r="O13" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="P13" s="134" t="s">
+      <c r="P13" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="Q13" s="134" t="s">
+      <c r="Q13" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="134" t="s">
+      <c r="R13" s="133" t="s">
         <v>114</v>
       </c>
-      <c r="S13" s="133" t="s">
+      <c r="S13" s="132" t="s">
         <v>117</v>
       </c>
-      <c r="T13" s="134" t="s">
+      <c r="T13" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="U13" s="134" t="s">
+      <c r="U13" s="133" t="s">
         <v>129</v>
       </c>
-      <c r="V13" s="134" t="s">
+      <c r="V13" s="133" t="s">
         <v>136</v>
       </c>
-      <c r="W13" s="133" t="s">
+      <c r="W13" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="X13" s="134" t="s">
+      <c r="X13" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="Y13" s="134" t="s">
+      <c r="Y13" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="Z13" s="133" t="s">
+      <c r="Z13" s="132" t="s">
         <v>95</v>
       </c>
-      <c r="AA13" s="130"/>
+      <c r="AA13" s="132" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="14" spans="1:27" ht="29.4" customHeight="1">
       <c r="A14" s="74">
@@ -22599,7 +22607,10 @@
         <f>IF(OR(D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D14&amp;F14="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G14*1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="130"/>
+      <c r="AA14" s="129">
+        <f>IF(F14="LTC1 Occupancy Control - Wall Mount (near or replacing wall switch)", 1, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:27" ht="29.4" customHeight="1">
       <c r="A15" s="74">
@@ -22680,7 +22691,10 @@
         <f t="shared" ref="Z15:Z78" si="14">IF(OR(D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D15&amp;F15="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G15*1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AA15" s="130"/>
+      <c r="AA15" s="129">
+        <f>IF(F15="LTC1 Occupancy Control - Wall Mount (near or replacing wall switch)", 1, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="29.4" customHeight="1">
       <c r="A16" s="74">
@@ -22756,7 +22770,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="130"/>
+      <c r="AA16" s="129">
+        <f t="shared" ref="AA15:AA78" si="15">IF(F16="LTC1 Occupancy Control - Wall Mount (near or replacing wall switch)", 1, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:27" ht="29.4" customHeight="1">
       <c r="A17" s="74">
@@ -22832,7 +22849,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="130"/>
+      <c r="AA17" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:27" ht="29.4" customHeight="1">
       <c r="A18" s="74">
@@ -22908,7 +22928,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA18" s="130"/>
+      <c r="AA18" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:27" ht="29.4" customHeight="1">
       <c r="A19" s="74">
@@ -22984,7 +23007,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="130"/>
+      <c r="AA19" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:27" ht="29.4" customHeight="1">
       <c r="A20" s="74">
@@ -23060,7 +23086,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA20" s="130"/>
+      <c r="AA20" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:27" ht="29.4" customHeight="1">
       <c r="A21" s="74">
@@ -23136,7 +23165,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA21" s="130"/>
+      <c r="AA21" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:27" ht="29.4" customHeight="1">
       <c r="A22" s="74">
@@ -23212,7 +23244,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA22" s="130"/>
+      <c r="AA22" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:27" ht="29.4" customHeight="1">
       <c r="A23" s="74">
@@ -23288,6 +23323,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA23" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:27" ht="29.4" customHeight="1">
       <c r="A24" s="74">
@@ -23363,6 +23402,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA24" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:27" ht="29.4" customHeight="1">
       <c r="A25" s="74">
@@ -23438,6 +23481,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA25" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:27" ht="29.4" customHeight="1" thickBot="1">
       <c r="A26" s="74">
@@ -23513,6 +23560,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA26" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A27" s="74">
@@ -23588,6 +23639,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA27" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A28" s="74">
@@ -23663,6 +23718,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA28" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A29" s="74">
@@ -23738,6 +23797,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA29" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A30" s="74">
@@ -23813,6 +23876,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA30" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A31" s="74">
@@ -23888,6 +23955,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA31" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A32" s="74">
@@ -23963,8 +24034,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA32" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="33" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A33" s="74">
         <v>20</v>
       </c>
@@ -24038,8 +24113,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA33" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="34" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A34" s="74">
         <v>21</v>
       </c>
@@ -24113,8 +24192,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA34" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="35" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A35" s="74">
         <v>22</v>
       </c>
@@ -24188,8 +24271,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA35" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="36" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A36" s="74">
         <v>23</v>
       </c>
@@ -24263,8 +24350,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA36" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="37" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A37" s="74">
         <v>24</v>
       </c>
@@ -24338,8 +24429,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA37" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="38" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A38" s="74">
         <v>25</v>
       </c>
@@ -24413,8 +24508,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA38" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="39" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A39" s="74">
         <v>26</v>
       </c>
@@ -24488,8 +24587,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA39" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="40" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A40" s="74">
         <v>27</v>
       </c>
@@ -24563,8 +24666,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA40" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="41" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A41" s="74">
         <v>28</v>
       </c>
@@ -24638,8 +24745,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA41" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="42" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A42" s="74">
         <v>29</v>
       </c>
@@ -24713,8 +24824,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA42" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="43" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A43" s="74">
         <v>30</v>
       </c>
@@ -24788,8 +24903,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA43" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="44" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A44" s="74">
         <v>31</v>
       </c>
@@ -24863,8 +24982,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA44" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="45" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A45" s="74">
         <v>32</v>
       </c>
@@ -24938,8 +25061,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA45" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="46" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A46" s="74">
         <v>33</v>
       </c>
@@ -25013,8 +25140,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA46" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="47" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A47" s="74">
         <v>34</v>
       </c>
@@ -25088,8 +25219,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA47" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="48" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A48" s="74">
         <v>35</v>
       </c>
@@ -25163,6 +25298,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA48" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A49" s="74">
@@ -25238,6 +25377,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA49" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A50" s="74">
@@ -25313,6 +25456,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA50" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A51" s="74">
@@ -25388,7 +25535,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AA51" s="130"/>
+      <c r="AA51" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A52" s="74">
@@ -25464,6 +25614,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA52" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A53" s="74">
@@ -25539,6 +25693,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA53" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A54" s="74">
@@ -25614,6 +25772,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA54" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A55" s="74">
@@ -25689,6 +25851,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA55" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A56" s="74">
@@ -25764,6 +25930,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA56" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A57" s="74">
@@ -25839,6 +26009,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA57" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A58" s="74">
@@ -25914,6 +26088,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA58" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A59" s="74">
@@ -25989,6 +26167,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA59" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A60" s="74">
@@ -26064,6 +26246,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA60" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A61" s="74">
@@ -26139,6 +26325,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA61" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A62" s="74">
@@ -26214,6 +26404,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA62" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A63" s="74">
@@ -26289,6 +26483,10 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA63" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A64" s="74">
@@ -26364,8 +26562,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA64" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="65" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A65" s="74">
         <v>52</v>
       </c>
@@ -26439,8 +26641,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA65" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="66" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A66" s="74">
         <v>53</v>
       </c>
@@ -26514,8 +26720,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA66" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="67" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A67" s="74">
         <v>54</v>
       </c>
@@ -26589,8 +26799,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA67" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="68" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A68" s="74">
         <v>55</v>
       </c>
@@ -26664,8 +26878,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA68" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="69" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A69" s="74">
         <v>56</v>
       </c>
@@ -26739,8 +26957,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA69" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="70" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A70" s="74">
         <v>57</v>
       </c>
@@ -26814,8 +27036,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA70" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="71" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A71" s="74">
         <v>58</v>
       </c>
@@ -26889,8 +27115,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA71" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="72" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A72" s="74">
         <v>59</v>
       </c>
@@ -26964,8 +27194,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA72" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="73" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A73" s="74">
         <v>60</v>
       </c>
@@ -27039,8 +27273,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA73" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="74" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A74" s="74">
         <v>61</v>
       </c>
@@ -27114,8 +27352,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA74" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="75" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A75" s="74">
         <v>62</v>
       </c>
@@ -27189,8 +27431,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA75" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="76" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A76" s="74">
         <v>63</v>
       </c>
@@ -27264,8 +27510,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA76" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="77" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A77" s="74">
         <v>64</v>
       </c>
@@ -27339,8 +27589,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA77" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:26" ht="29.4" hidden="1" customHeight="1">
+    <row r="78" spans="1:27" ht="29.4" hidden="1" customHeight="1">
       <c r="A78" s="74">
         <v>65</v>
       </c>
@@ -27414,8 +27668,12 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
+      <c r="AA78" s="129">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:26" ht="29.4" hidden="1" customHeight="1" thickBot="1">
+    <row r="79" spans="1:27" ht="29.4" hidden="1" customHeight="1" thickBot="1">
       <c r="A79" s="74">
         <v>66</v>
       </c>
@@ -27430,72 +27688,76 @@
       <c r="J79" s="90"/>
       <c r="K79" s="5"/>
       <c r="L79" s="81">
-        <f t="shared" ref="L79" si="15">IF(OR(D79&amp;F79="Interior CF 1L 13W QuadPAR 20 Integral LED Lamp ",D79&amp;F79="Interior CF 1L 23W QuadPAR 20 Integral LED Lamp ",D79&amp;F79="Halogen Incandescent, (1) 35W lampPAR 20 Integral LED Lamp ",D79&amp;F79="Halogen Incandescent, (1) 75W lampPAR 20 Integral LED Lamp ",D79&amp;F79="Incandescent, (1) 20W lampPAR 20 Integral LED Lamp "),1*G79,0)</f>
+        <f t="shared" ref="L79" si="16">IF(OR(D79&amp;F79="Interior CF 1L 13W QuadPAR 20 Integral LED Lamp ",D79&amp;F79="Interior CF 1L 23W QuadPAR 20 Integral LED Lamp ",D79&amp;F79="Halogen Incandescent, (1) 35W lampPAR 20 Integral LED Lamp ",D79&amp;F79="Halogen Incandescent, (1) 75W lampPAR 20 Integral LED Lamp ",D79&amp;F79="Incandescent, (1) 20W lampPAR 20 Integral LED Lamp "),1*G79,0)</f>
         <v>0</v>
       </c>
       <c r="M79" s="82">
-        <f t="shared" ref="M79" si="16">IF(D79&amp;F79="EXIT Incandescent, (1) 20W lampEXIT Sign, LED, (1) 2W lamp, Single Sided",1*G79, IF(D79&amp;F79="EXIT Incandescent, (2) 20W lampsEXIT Sign, LED, (2) 2W lamps, Dual Sided", 2*G79, 0))</f>
+        <f t="shared" ref="M79" si="17">IF(D79&amp;F79="EXIT Incandescent, (1) 20W lampEXIT Sign, LED, (1) 2W lamp, Single Sided",1*G79, IF(D79&amp;F79="EXIT Incandescent, (2) 20W lampsEXIT Sign, LED, (2) 2W lamps, Dual Sided", 2*G79, 0))</f>
         <v>0</v>
       </c>
       <c r="N79" s="1">
-        <f t="shared" ref="N79" si="17">IF(OR(D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", STD lampFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Standard BallastFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1, 0)</f>
+        <f t="shared" ref="N79" si="18">IF(OR(D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", STD lampFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Standard BallastFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="O79" s="1">
-        <f t="shared" ref="O79" si="18">IF(OR(D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"),1*G79,
+        <f t="shared" ref="O79" si="19">IF(OR(D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"),1*G79,
 IF(OR(D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"),2*G79,
 IF(OR(D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"),3*G79,
 IF(OR(D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)",D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)",D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"),4*G79,0))))</f>
         <v>0</v>
       </c>
       <c r="P79" s="1">
-        <f t="shared" ref="P79" si="19">IF(OR(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*6, 0)</f>
+        <f t="shared" ref="P79" si="20">IF(OR(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*6, 0)</f>
         <v>0</v>
       </c>
       <c r="Q79" s="1">
-        <f t="shared" ref="Q79" si="20">IF(D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)", G79*1, 0)</f>
+        <f t="shared" ref="Q79" si="21">IF(D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)", G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="R79" s="1">
-        <f t="shared" ref="R79" si="21">IF(OR(D79&amp;F79="Halogen Incandescent, (1) 100W lampInterior CF 1L 23W Quad",D79&amp;F79="Halogen Incandescent, (1) 75W lampInterior CF 1L 23W Quad",D79&amp;F79="Incandescent, (1) 100W lampInterior CF 1L 23W Quad",D79&amp;F79="Incandescent, (1) 90W lampInterior CF 1L 23W Quad"),G79*1,0)</f>
+        <f t="shared" ref="R79" si="22">IF(OR(D79&amp;F79="Halogen Incandescent, (1) 100W lampInterior CF 1L 23W Quad",D79&amp;F79="Halogen Incandescent, (1) 75W lampInterior CF 1L 23W Quad",D79&amp;F79="Incandescent, (1) 100W lampInterior CF 1L 23W Quad",D79&amp;F79="Incandescent, (1) 90W lampInterior CF 1L 23W Quad"),G79*1,0)</f>
         <v>0</v>
       </c>
       <c r="S79" s="1">
-        <f t="shared" ref="S79" si="22">IF(OR(D79&amp;F79="Halogen Incandescent, (1) 50W lampInterior CF 1L 13W Quad",D79&amp;F79="Halogen Incandescent, (1) 60W lampInterior CF 1L 13W Quad",D79&amp;F79="Incandescent, (1) 30W lampInterior CF 1L 13W Quad",D79&amp;F79="Incandescent, (1) 40W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 60W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 65W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 75W lampInterior CF 1L 13W Quad"),G79*1,0)</f>
+        <f t="shared" ref="S79" si="23">IF(OR(D79&amp;F79="Halogen Incandescent, (1) 50W lampInterior CF 1L 13W Quad",D79&amp;F79="Halogen Incandescent, (1) 60W lampInterior CF 1L 13W Quad",D79&amp;F79="Incandescent, (1) 30W lampInterior CF 1L 13W Quad",D79&amp;F79="Incandescent, (1) 40W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 60W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 65W lampInterior CF 1L 13W Quad", D79&amp;F79="Incandescent, (1) 75W lampInterior CF 1L 13W Quad"),G79*1,0)</f>
         <v>0</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" ref="T79" si="23">IF(OR(D79&amp;F79="Halogen, (1) Low Voltage MR16 lampMR 16 Integral LED Lamp", D79&amp;F79="Incandescent, (1) 25W lampMR 16 Integral LED Lamp"), G79*1, 0)</f>
+        <f t="shared" ref="T79" si="24">IF(OR(D79&amp;F79="Halogen, (1) Low Voltage MR16 lampMR 16 Integral LED Lamp", D79&amp;F79="Incandescent, (1) 25W lampMR 16 Integral LED Lamp"), G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" ref="U79" si="24">IF(D79&amp;F79="Incandescent, (1) 60W lampInterior CF 1L 13W Quad", G79*1, 0)</f>
+        <f t="shared" ref="U79" si="25">IF(D79&amp;F79="Incandescent, (1) 60W lampInterior CF 1L 13W Quad", G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="V79" s="1">
-        <f t="shared" ref="V79" si="25">IF(OR(D79&amp;F79="Metal Halide, (1) 350W lamp, Magnetic ballastFluorescent, (4) 45.8"&amp;CHAR(34)&amp;", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)", D79&amp;F79="Metal Halide, (1) 400W lamp, Magnetic ballastFluorescent, (4) 45.8"&amp;CHAR(34)&amp;", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)"), G79*1, 0)</f>
+        <f t="shared" ref="V79" si="26">IF(OR(D79&amp;F79="Metal Halide, (1) 350W lamp, Magnetic ballastFluorescent, (4) 45.8"&amp;CHAR(34)&amp;", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)", D79&amp;F79="Metal Halide, (1) 400W lamp, Magnetic ballastFluorescent, (4) 45.8"&amp;CHAR(34)&amp;", T-5 high-output lamps, (1) Programmed Rapid Start Ballast, HLO (.95 &lt; BF &lt; 1.1)"), G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="W79" s="1">
-        <f t="shared" ref="W79" si="26">IF(OR(D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", STD lampFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Standard BallastFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1, 0)</f>
+        <f t="shared" ref="W79" si="27">IF(OR(D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", STD lampFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Standard BallastFluorescent, (1) 24"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lamp, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (1) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1, 0)</f>
         <v>0</v>
       </c>
       <c r="X79" s="1">
-        <f t="shared" ref="X79" si="27">IF(OR(D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1,
+        <f t="shared" ref="X79" si="28">IF(OR(D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", ES lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)",D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (1) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&lt; 0.85)", D79&amp;F79="Fluorescent, (2) U-Tube, ES lampsFluorescent, (2) 6"&amp;CHAR(34)&amp;" spacing U-Tube, T-8 lamps, IS Ballast, NLO (0.85 &lt; BF &lt; 0.95)"), G79*1,
 IF(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", G79*2, 0))</f>
         <v>0</v>
       </c>
       <c r="Y79" s="1">
-        <f t="shared" ref="Y79" si="28">IF(OR(D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1,
+        <f t="shared" ref="Y79" si="29">IF(OR(D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (1) 96"&amp;CHAR(34)&amp;" ES lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (3) 48"&amp;CHAR(34)&amp;", T-8 lampFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (3) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 48"&amp;CHAR(34)&amp;", T-8 lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (2) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (2) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)"), G79*1,
 IF(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (6) 48"&amp;CHAR(34)&amp;", HPT8 32W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", G79*2, 0))</f>
         <v>0</v>
       </c>
       <c r="Z79" s="1">
-        <f t="shared" ref="Z79" si="29">IF(OR(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G79*1, 0)</f>
+        <f t="shared" ref="Z79" si="30">IF(OR(D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", ES lampsFluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)", D79&amp;F79="Fluorescent, (4) 96"&amp;CHAR(34)&amp;", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (4) 48"&amp;CHAR(34)&amp;", HPT8 28W lamp, Instant or Program Start Ballast, (&gt;/= 0.95)"), G79*1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA79" s="129">
+        <f t="shared" ref="AA79" si="31">IF(F79="LTC1 Occupancy Control - Wall Mount (near or replacing wall switch)", 1, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="19.2" customHeight="1" thickTop="1">
+    <row r="80" spans="1:27" ht="19.2" customHeight="1" thickTop="1">
       <c r="A80" s="93"/>
       <c r="B80" s="94" t="s">
         <v>17</v>
@@ -27510,64 +27772,68 @@
       </c>
       <c r="H80" s="95"/>
       <c r="I80" s="95"/>
-      <c r="L80" s="131">
+      <c r="L80" s="130">
         <f>SUM(L14:L79)</f>
         <v>0</v>
       </c>
-      <c r="M80" s="131">
-        <f t="shared" ref="M80:N80" si="30">SUM(M14:M79)</f>
-        <v>0</v>
-      </c>
-      <c r="N80" s="131">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O80" s="131">
-        <f t="shared" ref="O80:Z80" si="31">SUM(O14:O79)</f>
-        <v>0</v>
-      </c>
-      <c r="P80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="Q80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="R80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="S80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="T80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="U80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="V80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="W80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="X80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="Y80" s="131">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="Z80" s="131">
-        <f t="shared" si="31"/>
+      <c r="M80" s="130">
+        <f t="shared" ref="M80:N80" si="32">SUM(M14:M79)</f>
+        <v>0</v>
+      </c>
+      <c r="N80" s="130">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="O80" s="130">
+        <f t="shared" ref="O80:AA80" si="33">SUM(O14:O79)</f>
+        <v>0</v>
+      </c>
+      <c r="P80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="Q80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="T80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="U80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="V80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="X80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="Y80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="Z80" s="130">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AA80" s="130">
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -27614,29 +27880,29 @@
       <c r="K83" s="6"/>
     </row>
     <row r="84" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A84" s="155"/>
-      <c r="B84" s="156"/>
+      <c r="A84" s="165"/>
+      <c r="B84" s="166"/>
       <c r="C84" s="97"/>
       <c r="D84" s="97"/>
       <c r="E84" s="97"/>
-      <c r="F84" s="156"/>
-      <c r="G84" s="156"/>
+      <c r="F84" s="166"/>
+      <c r="G84" s="166"/>
       <c r="H84" s="97"/>
       <c r="I84" s="97"/>
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A85" s="145" t="s">
+      <c r="A85" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="146"/>
+      <c r="B85" s="157"/>
       <c r="C85" s="100"/>
       <c r="D85" s="100"/>
       <c r="E85" s="100"/>
-      <c r="F85" s="146" t="s">
+      <c r="F85" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="146"/>
+      <c r="G85" s="157"/>
       <c r="J85" s="7" t="s">
         <v>35</v>
       </c>
@@ -27651,10 +27917,10 @@
       <c r="E86" s="102"/>
       <c r="F86" s="102"/>
       <c r="G86" s="102"/>
-      <c r="J86" s="157" t="s">
+      <c r="J86" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="K86" s="158"/>
+      <c r="K86" s="145"/>
       <c r="L86" s="30"/>
     </row>
     <row r="87" spans="1:12" s="98" customFormat="1" ht="15" customHeight="1">
@@ -27665,40 +27931,40 @@
       <c r="E87" s="102"/>
       <c r="F87" s="102"/>
       <c r="G87" s="102"/>
-      <c r="J87" s="159"/>
-      <c r="K87" s="160"/>
+      <c r="J87" s="146"/>
+      <c r="K87" s="147"/>
       <c r="L87" s="30"/>
     </row>
     <row r="88" spans="1:12" s="98" customFormat="1" ht="22.95" customHeight="1" thickBot="1">
-      <c r="A88" s="153"/>
-      <c r="B88" s="154"/>
+      <c r="A88" s="163"/>
+      <c r="B88" s="164"/>
       <c r="C88" s="103"/>
       <c r="D88" s="103"/>
       <c r="E88" s="103"/>
-      <c r="F88" s="154"/>
-      <c r="G88" s="154"/>
+      <c r="F88" s="164"/>
+      <c r="G88" s="164"/>
       <c r="H88" s="97"/>
       <c r="I88" s="97"/>
-      <c r="J88" s="161" t="s">
+      <c r="J88" s="148" t="s">
         <v>34</v>
       </c>
-      <c r="K88" s="162"/>
+      <c r="K88" s="149"/>
       <c r="L88" s="104"/>
     </row>
     <row r="89" spans="1:12" s="98" customFormat="1" ht="17.399999999999999" customHeight="1">
-      <c r="A89" s="145" t="s">
+      <c r="A89" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="146"/>
+      <c r="B89" s="157"/>
       <c r="C89" s="100"/>
       <c r="D89" s="100"/>
       <c r="E89" s="100"/>
-      <c r="F89" s="146" t="s">
+      <c r="F89" s="157" t="s">
         <v>12</v>
       </c>
-      <c r="G89" s="146"/>
-      <c r="J89" s="163"/>
-      <c r="K89" s="164"/>
+      <c r="G89" s="157"/>
+      <c r="J89" s="150"/>
+      <c r="K89" s="151"/>
       <c r="L89" s="104"/>
     </row>
     <row r="90" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1">
@@ -27732,17 +27998,17 @@
       <c r="L91" s="110"/>
     </row>
     <row r="92" spans="1:12" s="98" customFormat="1" ht="25.2" customHeight="1" thickBot="1">
-      <c r="A92" s="149" t="s">
+      <c r="A92" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="B92" s="150"/>
+      <c r="B92" s="160"/>
       <c r="C92" s="111"/>
       <c r="D92" s="111"/>
       <c r="E92" s="111"/>
-      <c r="F92" s="150" t="s">
+      <c r="F92" s="160" t="s">
         <v>13</v>
       </c>
-      <c r="G92" s="150"/>
+      <c r="G92" s="160"/>
       <c r="H92" s="112"/>
       <c r="I92" s="113"/>
       <c r="J92" s="114" t="s">
@@ -27766,13 +28032,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J86:K87"/>
-    <mergeCell ref="J88:K89"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="J12:K12"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A92:B92"/>
@@ -27788,6 +28047,13 @@
     <mergeCell ref="F89:G89"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="F84:G84"/>
+    <mergeCell ref="J86:K87"/>
+    <mergeCell ref="J88:K89"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
@@ -27800,12 +28066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:S79"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -27852,7 +28116,7 @@
       <c r="P1" s="27"/>
       <c r="Q1" s="27"/>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:17">
       <c r="A2" s="122" t="s">
         <v>66</v>
       </c>
@@ -27873,7 +28137,7 @@
       <c r="G2" s="122"/>
       <c r="H2" s="98"/>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:17">
       <c r="A3" s="122" t="s">
         <v>69</v>
       </c>
@@ -27894,7 +28158,7 @@
       <c r="G3" s="122"/>
       <c r="H3" s="98"/>
     </row>
-    <row r="4" spans="1:17" hidden="1">
+    <row r="4" spans="1:17">
       <c r="A4" s="122" t="s">
         <v>70</v>
       </c>
@@ -27915,7 +28179,7 @@
       <c r="G4" s="122"/>
       <c r="H4" s="98"/>
     </row>
-    <row r="5" spans="1:17" hidden="1">
+    <row r="5" spans="1:17">
       <c r="A5" s="122" t="s">
         <v>73</v>
       </c>
@@ -27936,7 +28200,7 @@
       <c r="G5" s="122"/>
       <c r="H5" s="98"/>
     </row>
-    <row r="6" spans="1:17" hidden="1">
+    <row r="6" spans="1:17">
       <c r="A6" s="122" t="s">
         <v>75</v>
       </c>
@@ -27964,7 +28228,7 @@
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
     </row>
-    <row r="7" spans="1:17" hidden="1">
+    <row r="7" spans="1:17">
       <c r="A7" s="122" t="s">
         <v>79</v>
       </c>
@@ -27988,8 +28252,8 @@
         <v>1</v>
       </c>
       <c r="H7" s="98"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -28021,8 +28285,8 @@
         <v>1</v>
       </c>
       <c r="H8" s="98"/>
-      <c r="J8" s="130"/>
-      <c r="K8" s="130"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
@@ -28054,8 +28318,8 @@
         <v>1</v>
       </c>
       <c r="H9" s="98"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="129"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
@@ -28087,8 +28351,8 @@
         <v>1</v>
       </c>
       <c r="H10" s="98"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="129"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
@@ -28120,8 +28384,8 @@
         <v>1</v>
       </c>
       <c r="H11" s="98"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="130"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="129"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
@@ -28153,8 +28417,8 @@
         <v>1</v>
       </c>
       <c r="H12" s="98"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="130"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
@@ -28187,7 +28451,7 @@
       </c>
       <c r="H13" s="98"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="130"/>
+      <c r="K13" s="129"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
@@ -28220,7 +28484,7 @@
       </c>
       <c r="H14" s="98"/>
       <c r="J14" s="27"/>
-      <c r="K14" s="130"/>
+      <c r="K14" s="129"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
@@ -28261,7 +28525,7 @@
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
     </row>
-    <row r="16" spans="1:17" hidden="1">
+    <row r="16" spans="1:17">
       <c r="A16" s="122" t="s">
         <v>93</v>
       </c>
@@ -28294,7 +28558,7 @@
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
     </row>
-    <row r="17" spans="1:19" hidden="1">
+    <row r="17" spans="1:18">
       <c r="A17" s="122" t="s">
         <v>93</v>
       </c>
@@ -28319,7 +28583,7 @@
       </c>
       <c r="H17" s="98"/>
     </row>
-    <row r="18" spans="1:19" hidden="1">
+    <row r="18" spans="1:18">
       <c r="A18" s="122" t="s">
         <v>98</v>
       </c>
@@ -28344,7 +28608,7 @@
       </c>
       <c r="H18" s="98"/>
     </row>
-    <row r="19" spans="1:19" hidden="1">
+    <row r="19" spans="1:18">
       <c r="A19" s="122" t="s">
         <v>99</v>
       </c>
@@ -28377,7 +28641,7 @@
       <c r="P19" s="27"/>
       <c r="Q19" s="27"/>
     </row>
-    <row r="20" spans="1:19" hidden="1">
+    <row r="20" spans="1:18">
       <c r="A20" s="122" t="s">
         <v>100</v>
       </c>
@@ -28403,14 +28667,14 @@
       <c r="H20" s="98"/>
       <c r="J20" s="98"/>
       <c r="K20" s="98"/>
-      <c r="L20" s="130"/>
+      <c r="L20" s="129"/>
       <c r="M20" s="98"/>
       <c r="N20" s="98"/>
       <c r="O20" s="98"/>
       <c r="P20" s="98"/>
       <c r="Q20" s="27"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:18">
       <c r="A21" s="122" t="s">
         <v>101</v>
       </c>
@@ -28443,7 +28707,7 @@
       <c r="P21" s="27"/>
       <c r="Q21" s="27"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:18">
       <c r="A22" s="122" t="s">
         <v>102</v>
       </c>
@@ -28476,7 +28740,7 @@
       <c r="P22" s="27"/>
       <c r="Q22" s="27"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:18">
       <c r="A23" s="122" t="s">
         <v>103</v>
       </c>
@@ -28509,7 +28773,7 @@
       <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:18">
       <c r="A24" s="123" t="s">
         <v>104</v>
       </c>
@@ -28533,18 +28797,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="98"/>
-      <c r="Q24" s="143" t="s">
-        <v>104</v>
-      </c>
-      <c r="R24" s="144" t="s">
-        <v>142</v>
-      </c>
-      <c r="S24" s="26" t="str">
-        <f>Q24&amp;R24</f>
-        <v>Fluorescent, (4) 48", T-8 lamps, Instant Start Ballast, NLO (0.85 &lt; BF &lt; 0.95)Fluorescent, (3) 48", HPT8 28W lamp, Instant or Program Start Ballast, (0.85 &lt; BF &lt; 0.95)</v>
-      </c>
+      <c r="Q24" s="142"/>
+      <c r="R24" s="143"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:18">
       <c r="A25" s="122" t="s">
         <v>105</v>
       </c>
@@ -28569,11 +28825,11 @@
       </c>
       <c r="H25" s="98"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:18">
       <c r="A26" s="123" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="141" t="s">
+      <c r="B26" s="140" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="72" t="str">
@@ -28586,18 +28842,15 @@
       <c r="E26" s="123">
         <v>4</v>
       </c>
-      <c r="F26" s="142" t="s">
+      <c r="F26" s="141" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="122">
         <v>1</v>
       </c>
       <c r="H26" s="98"/>
-      <c r="R26" s="26" t="s">
-        <v>141</v>
-      </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:18">
       <c r="A27" s="122" t="s">
         <v>105</v>
       </c>
@@ -28621,11 +28874,8 @@
         <v>1</v>
       </c>
       <c r="H27" s="98"/>
-      <c r="R27" s="26" t="s">
-        <v>141</v>
-      </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:18">
       <c r="A28" s="123" t="s">
         <v>104</v>
       </c>
@@ -28650,7 +28900,7 @@
       </c>
       <c r="H28" s="98"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:18">
       <c r="A29" s="122" t="s">
         <v>105</v>
       </c>
@@ -28675,7 +28925,7 @@
       </c>
       <c r="H29" s="98"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:18">
       <c r="A30" s="122" t="s">
         <v>107</v>
       </c>
@@ -28700,7 +28950,7 @@
       </c>
       <c r="H30" s="98"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:18">
       <c r="A31" s="122" t="s">
         <v>107</v>
       </c>
@@ -28725,7 +28975,7 @@
       </c>
       <c r="H31" s="98"/>
     </row>
-    <row r="32" spans="1:19" hidden="1">
+    <row r="32" spans="1:18">
       <c r="A32" s="122" t="s">
         <v>108</v>
       </c>
@@ -28750,7 +29000,7 @@
       </c>
       <c r="H32" s="98"/>
     </row>
-    <row r="33" spans="1:8" hidden="1">
+    <row r="33" spans="1:8">
       <c r="A33" s="122" t="s">
         <v>108</v>
       </c>
@@ -28800,7 +29050,7 @@
       </c>
       <c r="H34" s="98"/>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" s="122" t="s">
         <v>113</v>
       </c>
@@ -28821,7 +29071,7 @@
       <c r="G35" s="122"/>
       <c r="H35" s="98"/>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" s="122" t="s">
         <v>115</v>
       </c>
@@ -28842,7 +29092,7 @@
       <c r="G36" s="122"/>
       <c r="H36" s="98"/>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" s="122" t="s">
         <v>116</v>
       </c>
@@ -28863,7 +29113,7 @@
       <c r="G37" s="122"/>
       <c r="H37" s="98"/>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" s="122" t="s">
         <v>118</v>
       </c>
@@ -28884,7 +29134,7 @@
       <c r="G38" s="122"/>
       <c r="H38" s="98"/>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" s="122" t="s">
         <v>119</v>
       </c>
@@ -28905,7 +29155,7 @@
       <c r="G39" s="122"/>
       <c r="H39" s="98"/>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" s="122" t="s">
         <v>119</v>
       </c>
@@ -28926,7 +29176,7 @@
       <c r="G40" s="122"/>
       <c r="H40" s="98"/>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" s="122" t="s">
         <v>120</v>
       </c>
@@ -28947,7 +29197,7 @@
       <c r="G41" s="122"/>
       <c r="H41" s="98"/>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" s="122" t="s">
         <v>123</v>
       </c>
@@ -28968,7 +29218,7 @@
       <c r="G42" s="122"/>
       <c r="H42" s="98"/>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" s="122" t="s">
         <v>124</v>
       </c>
@@ -28989,7 +29239,7 @@
       <c r="G43" s="122"/>
       <c r="H43" s="98"/>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44" s="122" t="s">
         <v>125</v>
       </c>
@@ -29010,7 +29260,7 @@
       <c r="G44" s="122"/>
       <c r="H44" s="98"/>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:8">
       <c r="A45" s="122" t="s">
         <v>126</v>
       </c>
@@ -29031,7 +29281,7 @@
       <c r="G45" s="122"/>
       <c r="H45" s="98"/>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46" s="122" t="s">
         <v>127</v>
       </c>
@@ -29052,7 +29302,7 @@
       <c r="G46" s="122"/>
       <c r="H46" s="98"/>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47" s="122" t="s">
         <v>128</v>
       </c>
@@ -29073,7 +29323,7 @@
       <c r="G47" s="122"/>
       <c r="H47" s="98"/>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48" s="122" t="s">
         <v>128</v>
       </c>
@@ -29096,7 +29346,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:8">
       <c r="A49" s="122" t="s">
         <v>131</v>
       </c>
@@ -29117,7 +29367,7 @@
       <c r="G49" s="122"/>
       <c r="H49" s="98"/>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50" s="122" t="s">
         <v>132</v>
       </c>
@@ -29138,7 +29388,7 @@
       <c r="G50" s="122"/>
       <c r="H50" s="98"/>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8">
       <c r="A51" s="122" t="s">
         <v>133</v>
       </c>
@@ -29159,7 +29409,7 @@
       <c r="G51" s="122"/>
       <c r="H51" s="98"/>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:8">
       <c r="A52" s="122" t="s">
         <v>134</v>
       </c>
@@ -29180,7 +29430,7 @@
       <c r="G52" s="122"/>
       <c r="H52" s="98"/>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53" s="122" t="s">
         <v>137</v>
       </c>
@@ -29201,7 +29451,7 @@
       <c r="G53" s="122"/>
       <c r="H53" s="98"/>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="C54" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29209,7 +29459,7 @@
       <c r="G54" s="98"/>
       <c r="H54" s="98"/>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="C55" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29217,14 +29467,14 @@
       <c r="G55" s="98"/>
       <c r="H55" s="98"/>
     </row>
-    <row r="56" spans="1:8" hidden="1">
+    <row r="56" spans="1:8">
       <c r="C56" s="72" t="s">
         <v>136</v>
       </c>
       <c r="G56" s="98"/>
       <c r="H56" s="98"/>
     </row>
-    <row r="57" spans="1:8" hidden="1">
+    <row r="57" spans="1:8">
       <c r="C57" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29232,7 +29482,7 @@
       <c r="G57" s="98"/>
       <c r="H57" s="98"/>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:8">
       <c r="C58" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29240,7 +29490,7 @@
       <c r="G58" s="98"/>
       <c r="H58" s="98"/>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="C59" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29248,7 +29498,7 @@
       <c r="G59" s="98"/>
       <c r="H59" s="98"/>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="C60" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29256,7 +29506,7 @@
       <c r="G60" s="98"/>
       <c r="H60" s="98"/>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="C61" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29264,7 +29514,7 @@
       <c r="G61" s="98"/>
       <c r="H61" s="98"/>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="C62" s="72" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -29299,36 +29549,22 @@
       <c r="C75" s="72"/>
     </row>
     <row r="76" spans="2:3">
-      <c r="C76" s="132"/>
+      <c r="C76" s="131"/>
     </row>
     <row r="79" spans="2:3">
       <c r="B79" s="72"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H62">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Sylvania QHE4X32T8/UNV ISL-SC"/>
-        <filter val="Sylvania QHE4X32T8/UNV ISN-SC"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV35"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:IV36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -29342,29 +29578,29 @@
   <sheetData>
     <row r="1" spans="1:4" ht="87" customHeight="1">
       <c r="A1" s="124"/>
-      <c r="B1" s="171" t="s">
+      <c r="B1" s="190" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="172"/>
-      <c r="D1" s="173"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="192"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="172" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="176" t="s">
+      <c r="B2" s="174"/>
+      <c r="C2" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="177"/>
+      <c r="D2" s="189"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="178"/>
-      <c r="B3" s="179"/>
-      <c r="C3" s="180" t="s">
+      <c r="A3" s="181"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="187" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="177"/>
+      <c r="D3" s="189"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="17" t="s">
@@ -29381,321 +29617,311 @@
         <f>IF('Audit Master'!L80=0, "", 'Audit Master'!L80)</f>
         <v/>
       </c>
-      <c r="B5" s="168" t="str">
+      <c r="B5" s="184" t="str">
         <f>IF(A5="", "", "Philips 40820-3")</f>
         <v/>
       </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="170"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="186"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="125" t="str">
         <f>IF('Audit Master'!M80=0, "", 'Audit Master'!M80)</f>
         <v/>
       </c>
-      <c r="B6" s="168" t="str">
+      <c r="B6" s="184" t="str">
         <f>IF(A6="", "", "TCP 20714")</f>
         <v/>
       </c>
-      <c r="C6" s="169"/>
-      <c r="D6" s="170"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="186"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="125" t="str">
         <f>IF('Audit Master'!N80=0, "", 'Audit Master'!N80)</f>
         <v/>
       </c>
-      <c r="B7" s="168" t="str">
+      <c r="B7" s="184" t="str">
         <f>IF(A7="", "", "Sylvania F017XP")</f>
         <v/>
       </c>
-      <c r="C7" s="169"/>
-      <c r="D7" s="170"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="186"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="126" t="str">
         <f>IF('Audit Master'!O80=0, "", 'Audit Master'!O80)</f>
         <v/>
       </c>
-      <c r="B8" s="168" t="str">
+      <c r="B8" s="184" t="str">
         <f>IF(A8="", "", "Sylvania F028SS")</f>
         <v/>
       </c>
-      <c r="C8" s="169"/>
-      <c r="D8" s="170"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="186"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="126" t="str">
         <f>IF('Audit Master'!P80=0, "", 'Audit Master'!P80)</f>
         <v/>
       </c>
-      <c r="B9" s="168" t="str">
+      <c r="B9" s="184" t="str">
         <f>IF(A9="", "", "Sylvania F032XP")</f>
         <v/>
       </c>
-      <c r="C9" s="169"/>
-      <c r="D9" s="170"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="186"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="126" t="str">
         <f>IF('Audit Master'!Q80=0, "", 'Audit Master'!Q80)</f>
         <v/>
       </c>
-      <c r="B10" s="168" t="str">
+      <c r="B10" s="184" t="str">
         <f>IF(A10="", "", "Sylvania FB030")</f>
         <v/>
       </c>
-      <c r="C10" s="169"/>
-      <c r="D10" s="170"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="186"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="126" t="str">
         <f>IF('Audit Master'!R80=0, "", 'Audit Master'!R80)</f>
         <v/>
       </c>
-      <c r="B11" s="168" t="str">
+      <c r="B11" s="184" t="str">
         <f>IF(A11="", "", "TCP 33123SP")</f>
         <v/>
       </c>
-      <c r="C11" s="169"/>
-      <c r="D11" s="170"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="186"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="126" t="str">
         <f>IF('Audit Master'!S80=0, "", 'Audit Master'!S80)</f>
         <v/>
       </c>
-      <c r="B12" s="168" t="str">
+      <c r="B12" s="184" t="str">
         <f>IF(A12="", "", "TCP 33113SP")</f>
         <v/>
       </c>
-      <c r="C12" s="169"/>
-      <c r="D12" s="170"/>
+      <c r="C12" s="185"/>
+      <c r="D12" s="186"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="126" t="str">
         <f>IF('Audit Master'!T80=0, "", 'Audit Master'!T80)</f>
         <v/>
       </c>
-      <c r="B13" s="168" t="str">
+      <c r="B13" s="184" t="str">
         <f>IF(A13="", "", "Philips 40877-3")</f>
         <v/>
       </c>
-      <c r="C13" s="169"/>
-      <c r="D13" s="170"/>
+      <c r="C13" s="185"/>
+      <c r="D13" s="186"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="126" t="str">
         <f>IF('Audit Master'!U80=0, "", 'Audit Master'!U80)</f>
         <v/>
       </c>
-      <c r="B14" s="168" t="str">
+      <c r="B14" s="184" t="str">
         <f>IF(A14="", "", "TCP 33213SSP")</f>
         <v/>
       </c>
-      <c r="C14" s="169"/>
-      <c r="D14" s="170"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="186"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="126" t="str">
         <f>IF('Audit Master'!V80=0, "", 'Audit Master'!V80)</f>
         <v/>
       </c>
-      <c r="B15" s="168" t="str">
+      <c r="B15" s="184" t="str">
         <f>IF(A15="", "", "Sylvania FP54T5HO")</f>
         <v/>
       </c>
-      <c r="C15" s="169"/>
-      <c r="D15" s="170"/>
+      <c r="C15" s="185"/>
+      <c r="D15" s="186"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="127" t="str">
         <f>IF('Audit Master'!W80=0, "", 'Audit Master'!W80)</f>
         <v/>
       </c>
-      <c r="B16" s="168" t="str">
+      <c r="B16" s="184" t="str">
         <f>IF(A16="", "", "Sylvania QHE2X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C16" s="169"/>
-      <c r="D16" s="170"/>
+      <c r="C16" s="185"/>
+      <c r="D16" s="186"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="126" t="str">
         <f>IF('Audit Master'!X80=0, "", 'Audit Master'!X80)</f>
         <v/>
       </c>
-      <c r="B17" s="168" t="str">
+      <c r="B17" s="184" t="str">
         <f>IF(A17="", "", "Sylvania QHE4X32T8/UNV ISL-SC")</f>
         <v/>
       </c>
-      <c r="C17" s="169"/>
-      <c r="D17" s="170"/>
+      <c r="C17" s="185"/>
+      <c r="D17" s="186"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="126" t="str">
         <f>IF('Audit Master'!Y80=0, "", 'Audit Master'!Y80)</f>
         <v/>
       </c>
-      <c r="B18" s="168" t="str">
+      <c r="B18" s="184" t="str">
         <f>IF(A18="", "", "Sylvania QHE4X32T8/UNV ISN-SC")</f>
         <v/>
       </c>
-      <c r="C18" s="169"/>
-      <c r="D18" s="170"/>
+      <c r="C18" s="185"/>
+      <c r="D18" s="186"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="128" t="str">
+      <c r="A19" s="126" t="str">
         <f>IF('Audit Master'!Z80=0, "", 'Audit Master'!Z80)</f>
         <v/>
       </c>
-      <c r="B19" s="168" t="str">
+      <c r="B19" s="184" t="str">
         <f>IF(A19="", "", "Sylvania QHE4X32T8/UNV ISH")</f>
         <v/>
       </c>
-      <c r="C19" s="169"/>
-      <c r="D19" s="170"/>
+      <c r="C19" s="185"/>
+      <c r="D19" s="186"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="180"/>
-      <c r="B20" s="176"/>
-      <c r="C20" s="176"/>
-      <c r="D20" s="177"/>
+      <c r="A20" s="126" t="str">
+        <f>IF('Audit Master'!AA80=0, "", 'Audit Master'!AA80)</f>
+        <v/>
+      </c>
+      <c r="B20" s="184" t="str">
+        <f>IF(A20="", "", "LTC1 Occupancy Control - Wall Mount")</f>
+        <v/>
+      </c>
+      <c r="C20" s="185"/>
+      <c r="D20" s="186"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="184" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="185"/>
-      <c r="C21" s="185"/>
-      <c r="D21" s="186"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="188"/>
+      <c r="D21" s="189"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="187"/>
-      <c r="B22" s="188"/>
-      <c r="C22" s="188"/>
-      <c r="D22" s="189"/>
+      <c r="A22" s="178" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="179"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="180"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="187"/>
-      <c r="B23" s="188"/>
-      <c r="C23" s="188"/>
-      <c r="D23" s="189"/>
+      <c r="A23" s="167"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="168"/>
+      <c r="D23" s="169"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="181"/>
-      <c r="B24" s="182"/>
-      <c r="C24" s="182"/>
-      <c r="D24" s="183"/>
+      <c r="A24" s="167"/>
+      <c r="B24" s="168"/>
+      <c r="C24" s="168"/>
+      <c r="D24" s="169"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="174" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="192"/>
-      <c r="C25" s="192"/>
-      <c r="D25" s="175"/>
+      <c r="A25" s="175"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="177"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="181"/>
-      <c r="B26" s="182"/>
-      <c r="C26" s="182"/>
-      <c r="D26" s="183"/>
+      <c r="A26" s="172" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="173"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="174"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="174" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="192"/>
-      <c r="C27" s="192"/>
-      <c r="D27" s="175"/>
+      <c r="A27" s="175"/>
+      <c r="B27" s="176"/>
+      <c r="C27" s="176"/>
+      <c r="D27" s="177"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="184"/>
-      <c r="B28" s="185"/>
-      <c r="C28" s="185"/>
-      <c r="D28" s="186"/>
+      <c r="A28" s="172" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="173"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="174"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="178"/>
-      <c r="B29" s="193"/>
-      <c r="C29" s="193"/>
-      <c r="D29" s="179"/>
+      <c r="B29" s="179"/>
+      <c r="C29" s="179"/>
+      <c r="D29" s="180"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="174" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="192"/>
-      <c r="C30" s="192"/>
-      <c r="D30" s="175"/>
+      <c r="A30" s="181"/>
+      <c r="B30" s="182"/>
+      <c r="C30" s="182"/>
+      <c r="D30" s="183"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="187"/>
-      <c r="B31" s="188"/>
-      <c r="C31" s="188"/>
-      <c r="D31" s="189"/>
+      <c r="A31" s="172" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="173"/>
+      <c r="C31" s="173"/>
+      <c r="D31" s="174"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="187"/>
-      <c r="B32" s="188"/>
-      <c r="C32" s="188"/>
-      <c r="D32" s="189"/>
+    <row r="32" spans="1:4">
+      <c r="A32" s="167"/>
+      <c r="B32" s="168"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="169"/>
     </row>
-    <row r="33" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A33" s="190" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A33" s="167"/>
+      <c r="B33" s="168"/>
+      <c r="C33" s="168"/>
+      <c r="D33" s="169"/>
+    </row>
+    <row r="34" spans="1:4" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A34" s="170" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="191"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22" t="s">
+      <c r="B34" s="171"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21" customHeight="1" thickBot="1">
-      <c r="A34" s="23" t="s">
+    <row r="35" spans="1:4" ht="21" customHeight="1" thickBot="1">
+      <c r="A35" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25" t="s">
+      <c r="B35" s="24"/>
+      <c r="C35" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="24"/>
+      <c r="D35" s="24"/>
     </row>
-    <row r="35" spans="1:4" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A35" s="23" t="s">
+    <row r="36" spans="1:4" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A36" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="129"/>
-      <c r="C35" s="25" t="s">
+      <c r="B36" s="128"/>
+      <c r="C36" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="129"/>
+      <c r="D36" s="128"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="B18:D18"/>
+  <mergeCells count="35">
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A2:B2"/>
@@ -29708,8 +29934,32 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>